<commit_message>
push output for 7/14 with updated code
</commit_message>
<xml_diff>
--- a/combined-datasets/state.xlsx
+++ b/combined-datasets/state.xlsx
@@ -168,7 +168,7 @@
     <t xml:space="preserve">Death_Investigations</t>
   </si>
   <si>
-    <t xml:space="preserve">136419</t>
+    <t xml:space="preserve">142397.79999999999</t>
   </si>
 </sst>
 </file>
@@ -8430,7 +8430,7 @@
         <v>1117274</v>
       </c>
       <c r="S92" t="n">
-        <v>0.0662</v>
+        <v>0.06623691212093</v>
       </c>
       <c r="T92" t="n">
         <v>21585</v>
@@ -8550,7 +8550,7 @@
         <v>1150868</v>
       </c>
       <c r="S93" t="n">
-        <v>0.0626</v>
+        <v>0.06259941815807</v>
       </c>
       <c r="T93" t="n">
         <v>23620</v>
@@ -8670,7 +8670,7 @@
         <v>1174948</v>
       </c>
       <c r="S94" t="n">
-        <v>0.0603</v>
+        <v>0.06027296332167</v>
       </c>
       <c r="T94" t="n">
         <v>24043</v>
@@ -8790,7 +8790,7 @@
         <v>1209187</v>
       </c>
       <c r="S95" t="n">
-        <v>0.0644</v>
+        <v>0.06437848992474</v>
       </c>
       <c r="T95" t="n">
         <v>23537</v>
@@ -8910,7 +8910,7 @@
         <v>1218955</v>
       </c>
       <c r="S96" t="n">
-        <v>0.08</v>
+        <v>0.08002311858263</v>
       </c>
       <c r="T96" t="n">
         <v>20021</v>
@@ -9150,7 +9150,7 @@
         <v>1286139</v>
       </c>
       <c r="S98" t="n">
-        <v>0.0666</v>
+        <v>0.06662901614215</v>
       </c>
       <c r="T98" t="n">
         <v>23019</v>
@@ -9270,7 +9270,7 @@
         <v>1302049</v>
       </c>
       <c r="S99" t="n">
-        <v>0.0692</v>
+        <v>0.06923969180723</v>
       </c>
       <c r="T99" t="n">
         <v>22046</v>
@@ -9386,7 +9386,7 @@
         <v>1348893</v>
       </c>
       <c r="S100" t="n">
-        <v>0.0685</v>
+        <v>0.06846481685691</v>
       </c>
       <c r="T100" t="n">
         <v>23966</v>
@@ -9504,7 +9504,7 @@
         <v>1370131</v>
       </c>
       <c r="S101" t="n">
-        <v>0.0705</v>
+        <v>0.07052200676015</v>
       </c>
       <c r="T101" t="n">
         <v>23626</v>
@@ -9624,7 +9624,7 @@
         <v>1404369</v>
       </c>
       <c r="S102" t="n">
-        <v>0.0722</v>
+        <v>0.07223931705799</v>
       </c>
       <c r="T102" t="n">
         <v>23863</v>
@@ -9744,7 +9744,7 @@
         <v>1442950</v>
       </c>
       <c r="S103" t="n">
-        <v>0.0611</v>
+        <v>0.06107731000976</v>
       </c>
       <c r="T103" t="n">
         <v>29139</v>
@@ -9984,7 +9984,7 @@
         <v>1499015</v>
       </c>
       <c r="S105" t="n">
-        <v>0.0671</v>
+        <v>0.06709533684425</v>
       </c>
       <c r="T105" t="n">
         <v>28727</v>
@@ -10104,7 +10104,7 @@
         <v>1522434</v>
       </c>
       <c r="S106" t="n">
-        <v>0.0694</v>
+        <v>0.06941707304209</v>
       </c>
       <c r="T106" t="n">
         <v>29793</v>
@@ -10224,7 +10224,7 @@
         <v>1560537</v>
       </c>
       <c r="S107" t="n">
-        <v>0.075</v>
+        <v>0.07497728638027</v>
       </c>
       <c r="T107" t="n">
         <v>28774</v>
@@ -10464,7 +10464,7 @@
         <v>1622851</v>
       </c>
       <c r="S109" t="n">
-        <v>0.0894</v>
+        <v>0.08936916175479</v>
       </c>
       <c r="T109" t="n">
         <v>29011</v>
@@ -10584,7 +10584,7 @@
         <v>1690124</v>
       </c>
       <c r="S110" t="n">
-        <v>0.088</v>
+        <v>0.08795944343323</v>
       </c>
       <c r="T110" t="n">
         <v>32885</v>
@@ -10824,7 +10824,7 @@
         <v>1767701</v>
       </c>
       <c r="S112" t="n">
-        <v>0.0964</v>
+        <v>0.09640261560072</v>
       </c>
       <c r="T112" t="n">
         <v>35550</v>
@@ -10940,7 +10940,7 @@
         <v>1805642</v>
       </c>
       <c r="S113" t="n">
-        <v>0.1042</v>
+        <v>0.10422837848208</v>
       </c>
       <c r="T113" t="n">
         <v>37231</v>
@@ -11060,7 +11060,7 @@
         <v>1836037</v>
       </c>
       <c r="S114" t="n">
-        <v>0.1176</v>
+        <v>0.11759188232068</v>
       </c>
       <c r="T114" t="n">
         <v>35943</v>
@@ -11180,7 +11180,7 @@
         <v>1875197</v>
       </c>
       <c r="S115" t="n">
-        <v>0.1173</v>
+        <v>0.11727744861385</v>
       </c>
       <c r="T115" t="n">
         <v>39060</v>
@@ -11300,7 +11300,7 @@
         <v>1903661</v>
       </c>
       <c r="S116" t="n">
-        <v>0.1323</v>
+        <v>0.13228718565459</v>
       </c>
       <c r="T116" t="n">
         <v>37061</v>
@@ -11420,7 +11420,7 @@
         <v>1959617</v>
       </c>
       <c r="S117" t="n">
-        <v>0.1431</v>
+        <v>0.14309405354181</v>
       </c>
       <c r="T117" t="n">
         <v>35577</v>
@@ -11540,7 +11540,7 @@
         <v>2006724</v>
       </c>
       <c r="S118" t="n">
-        <v>0.1374</v>
+        <v>0.13739729069509</v>
       </c>
       <c r="T118" t="n">
         <v>38597</v>
@@ -11660,7 +11660,7 @@
         <v>2061939</v>
       </c>
       <c r="S119" t="n">
-        <v>0.1402</v>
+        <v>0.14018794670431</v>
       </c>
       <c r="T119" t="n">
         <v>38856</v>
@@ -11780,7 +11780,7 @@
         <v>2119036</v>
       </c>
       <c r="S120" t="n">
-        <v>0.1358</v>
+        <v>0.13581542048065</v>
       </c>
       <c r="T120" t="n">
         <v>41670</v>
@@ -11900,7 +11900,7 @@
         <v>2174548</v>
       </c>
       <c r="S121" t="n">
-        <v>0.1332</v>
+        <v>0.13316248660981</v>
       </c>
       <c r="T121" t="n">
         <v>45209</v>
@@ -12022,7 +12022,7 @@
         <v>2212947</v>
       </c>
       <c r="S122" t="n">
-        <v>0.1392</v>
+        <v>0.13917844913637</v>
       </c>
       <c r="T122" t="n">
         <v>45225</v>
@@ -12144,7 +12144,7 @@
         <v>2273591</v>
       </c>
       <c r="S123" t="n">
-        <v>0.1315</v>
+        <v>0.13154795505798</v>
       </c>
       <c r="T123" t="n">
         <v>49855</v>
@@ -12266,7 +12266,7 @@
         <v>2338098</v>
       </c>
       <c r="S124" t="n">
-        <v>0.1352</v>
+        <v>0.13517270641306</v>
       </c>
       <c r="T124" t="n">
         <v>51177</v>
@@ -12388,7 +12388,7 @@
         <v>2371709</v>
       </c>
       <c r="S125" t="n">
-        <v>0.135</v>
+        <v>0.13500899750392</v>
       </c>
       <c r="T125" t="n">
         <v>49220</v>
@@ -12510,7 +12510,7 @@
         <v>2431861</v>
       </c>
       <c r="S126" t="n">
-        <v>0.1351</v>
+        <v>0.13507194500078</v>
       </c>
       <c r="T126" t="n">
         <v>50286</v>
@@ -12632,7 +12632,7 @@
         <v>2471029</v>
       </c>
       <c r="S127" t="n">
-        <v>0.1503</v>
+        <v>0.15025240527379</v>
       </c>
       <c r="T127" t="n">
         <v>48109</v>
@@ -12754,7 +12754,7 @@
         <v>2526940</v>
       </c>
       <c r="S128" t="n">
-        <v>0.1556</v>
+        <v>0.15560343677851</v>
       </c>
       <c r="T128" t="n">
         <v>48201</v>
@@ -12876,7 +12876,7 @@
         <v>2603903</v>
       </c>
       <c r="S129" t="n">
-        <v>0.1446</v>
+        <v>0.14464341297691</v>
       </c>
       <c r="T129" t="n">
         <v>53698</v>
@@ -12998,7 +12998,7 @@
         <v>2644496</v>
       </c>
       <c r="S130" t="n">
-        <v>0.1581</v>
+        <v>0.15812361136341</v>
       </c>
       <c r="T130" t="n">
         <v>51116</v>
@@ -13120,7 +13120,7 @@
         <v>2710290</v>
       </c>
       <c r="S131" t="n">
-        <v>0.1633</v>
+        <v>0.16329665986635</v>
       </c>
       <c r="T131" t="n">
         <v>51328</v>
@@ -13242,7 +13242,7 @@
         <v>2757859</v>
       </c>
       <c r="S132" t="n">
-        <v>0.1685</v>
+        <v>0.16849010085123</v>
       </c>
       <c r="T132" t="n">
         <v>53771</v>
@@ -13324,10 +13324,18 @@
       <c r="E133" t="n">
         <v>43</v>
       </c>
-      <c r="F133"/>
-      <c r="G133"/>
-      <c r="H133"/>
-      <c r="I133"/>
+      <c r="F133" t="n">
+        <v>2205822</v>
+      </c>
+      <c r="G133" t="n">
+        <v>40199</v>
+      </c>
+      <c r="H133" t="n">
+        <v>134345</v>
+      </c>
+      <c r="I133" t="n">
+        <v>-2796</v>
+      </c>
       <c r="J133" t="e">
         <v>#NUM!</v>
       </c>
@@ -13346,18 +13354,28 @@
       <c r="O133" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="P133"/>
-      <c r="Q133"/>
+      <c r="P133" t="n">
+        <v>2598680</v>
+      </c>
+      <c r="Q133" t="n">
+        <v>222123</v>
+      </c>
       <c r="R133" t="n">
         <v>2820803</v>
       </c>
-      <c r="S133"/>
-      <c r="T133"/>
-      <c r="U133"/>
-      <c r="V133"/>
-      <c r="W133" t="n">
-        <v>10405</v>
-      </c>
+      <c r="S133" t="n">
+        <v>0.16893795062442</v>
+      </c>
+      <c r="T133" t="n">
+        <v>53913</v>
+      </c>
+      <c r="U133" t="n">
+        <v>1650</v>
+      </c>
+      <c r="V133" t="n">
+        <v>55563</v>
+      </c>
+      <c r="W133"/>
       <c r="X133" t="n">
         <v>379</v>
       </c>
@@ -13407,6 +13425,106 @@
         <v>5245</v>
       </c>
       <c r="AN133" t="n">
+        <v>29677668</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" s="1" t="n">
+        <v>44026</v>
+      </c>
+      <c r="B134" t="n">
+        <v>275058</v>
+      </c>
+      <c r="C134" t="n">
+        <v>10745</v>
+      </c>
+      <c r="D134" t="n">
+        <v>3322</v>
+      </c>
+      <c r="E134" t="n">
+        <v>87</v>
+      </c>
+      <c r="F134"/>
+      <c r="G134"/>
+      <c r="H134"/>
+      <c r="I134"/>
+      <c r="J134" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="K134" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="L134" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="M134" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="N134" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="O134" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="P134"/>
+      <c r="Q134"/>
+      <c r="R134" t="n">
+        <v>2864541</v>
+      </c>
+      <c r="S134"/>
+      <c r="T134"/>
+      <c r="U134"/>
+      <c r="V134"/>
+      <c r="W134"/>
+      <c r="X134" t="n">
+        <v>386</v>
+      </c>
+      <c r="Y134" t="n">
+        <v>1163</v>
+      </c>
+      <c r="Z134" t="n">
+        <v>173</v>
+      </c>
+      <c r="AA134" t="n">
+        <v>374</v>
+      </c>
+      <c r="AB134" t="n">
+        <v>838</v>
+      </c>
+      <c r="AC134" t="n">
+        <v>9231</v>
+      </c>
+      <c r="AD134" t="n">
+        <v>1173</v>
+      </c>
+      <c r="AE134" t="n">
+        <v>3371</v>
+      </c>
+      <c r="AF134" t="n">
+        <v>10569</v>
+      </c>
+      <c r="AG134" t="n">
+        <v>7425</v>
+      </c>
+      <c r="AH134" t="n">
+        <v>3144</v>
+      </c>
+      <c r="AI134" t="n">
+        <v>11402</v>
+      </c>
+      <c r="AJ134" t="n">
+        <v>949</v>
+      </c>
+      <c r="AK134" t="n">
+        <v>43615</v>
+      </c>
+      <c r="AL134" t="n">
+        <v>6334</v>
+      </c>
+      <c r="AM134" t="n">
+        <v>5051</v>
+      </c>
+      <c r="AN134" t="n">
         <v>29677668</v>
       </c>
     </row>
@@ -13464,34 +13582,34 @@
         <v>51</v>
       </c>
       <c r="B2" t="n">
-        <v>124659</v>
+        <v>129338</v>
       </c>
       <c r="C2" t="n">
-        <v>106350</v>
+        <v>106892</v>
       </c>
       <c r="D2" t="n">
-        <v>2714453</v>
+        <v>2757649</v>
       </c>
       <c r="E2" t="n">
-        <v>7542</v>
+        <v>7646</v>
       </c>
       <c r="F2" t="n">
-        <v>55632</v>
+        <v>55017</v>
       </c>
       <c r="G2" t="n">
-        <v>12066</v>
+        <v>11402</v>
       </c>
       <c r="H2" t="n">
-        <v>984</v>
+        <v>949</v>
       </c>
       <c r="I2" t="n">
-        <v>5245</v>
+        <v>5051</v>
       </c>
       <c r="J2" t="n">
-        <v>25465</v>
+        <v>25496</v>
       </c>
       <c r="K2" t="n">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add adjustment for DSHS death reporting change
</commit_message>
<xml_diff>
--- a/combined-datasets/state.xlsx
+++ b/combined-datasets/state.xlsx
@@ -7242,10 +7242,10 @@
         <v>0</v>
       </c>
       <c r="D65" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E65" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F65" t="n">
         <v>0</v>
@@ -7373,7 +7373,7 @@
         <v>0</v>
       </c>
       <c r="D66" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E66" t="n">
         <v>0</v>
@@ -7504,7 +7504,7 @@
         <v>5</v>
       </c>
       <c r="D67" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E67" t="n">
         <v>0</v>
@@ -7638,7 +7638,7 @@
         <v>1</v>
       </c>
       <c r="E68" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F68" t="n">
         <v>0</v>
@@ -8290,10 +8290,10 @@
         <v>4</v>
       </c>
       <c r="D73" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E73" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F73" t="n">
         <v>0</v>
@@ -8421,10 +8421,10 @@
         <v>0</v>
       </c>
       <c r="D74" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E74" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F74" t="n">
         <v>0</v>
@@ -8552,10 +8552,10 @@
         <v>0</v>
       </c>
       <c r="D75" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E75" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F75" t="n">
         <v>0</v>
@@ -8683,10 +8683,10 @@
         <v>34</v>
       </c>
       <c r="D76" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E76" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F76" t="n">
         <v>0</v>
@@ -8814,10 +8814,10 @@
         <v>0</v>
       </c>
       <c r="D77" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E77" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F77" t="n">
         <v>0</v>
@@ -8945,10 +8945,10 @@
         <v>7</v>
       </c>
       <c r="D78" t="n">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E78" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F78" t="n">
         <v>0</v>
@@ -9076,7 +9076,7 @@
         <v>19</v>
       </c>
       <c r="D79" t="n">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E79" t="n">
         <v>2</v>
@@ -9207,10 +9207,10 @@
         <v>26</v>
       </c>
       <c r="D80" t="n">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E80" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F80" t="n">
         <v>0</v>
@@ -9338,10 +9338,10 @@
         <v>67</v>
       </c>
       <c r="D81" t="n">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="E81" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F81" t="n">
         <v>0</v>
@@ -9469,10 +9469,10 @@
         <v>60</v>
       </c>
       <c r="D82" t="n">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="E82" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F82" t="n">
         <v>0</v>
@@ -9600,10 +9600,10 @@
         <v>28</v>
       </c>
       <c r="D83" t="n">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="E83" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="F83" t="n">
         <v>0</v>
@@ -9731,10 +9731,10 @@
         <v>24</v>
       </c>
       <c r="D84" t="n">
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="E84" t="n">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="F84" t="n">
         <v>0</v>
@@ -9862,10 +9862,10 @@
         <v>425</v>
       </c>
       <c r="D85" t="n">
-        <v>48</v>
+        <v>22</v>
       </c>
       <c r="E85" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F85" t="n">
         <v>0</v>
@@ -9993,10 +9993,10 @@
         <v>263</v>
       </c>
       <c r="D86" t="n">
-        <v>60</v>
+        <v>28</v>
       </c>
       <c r="E86" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="F86" t="n">
         <v>0</v>
@@ -10124,10 +10124,10 @@
         <v>419</v>
       </c>
       <c r="D87" t="n">
-        <v>72</v>
+        <v>39</v>
       </c>
       <c r="E87" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F87" t="n">
         <v>0</v>
@@ -10255,10 +10255,10 @@
         <v>337</v>
       </c>
       <c r="D88" t="n">
-        <v>90</v>
+        <v>48</v>
       </c>
       <c r="E88" t="n">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="F88" t="n">
         <v>0</v>
@@ -10386,10 +10386,10 @@
         <v>317</v>
       </c>
       <c r="D89" t="n">
-        <v>103</v>
+        <v>60</v>
       </c>
       <c r="E89" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F89" t="n">
         <v>0</v>
@@ -10517,10 +10517,10 @@
         <v>504</v>
       </c>
       <c r="D90" t="n">
-        <v>125</v>
+        <v>72</v>
       </c>
       <c r="E90" t="n">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="F90" t="n">
         <v>0</v>
@@ -10648,10 +10648,10 @@
         <v>322</v>
       </c>
       <c r="D91" t="n">
-        <v>148</v>
+        <v>90</v>
       </c>
       <c r="E91" t="n">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="F91" t="n">
         <v>0</v>
@@ -10779,10 +10779,10 @@
         <v>392</v>
       </c>
       <c r="D92" t="n">
-        <v>168</v>
+        <v>103</v>
       </c>
       <c r="E92" t="n">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="F92" t="n">
         <v>0</v>
@@ -10910,10 +10910,10 @@
         <v>730</v>
       </c>
       <c r="D93" t="n">
-        <v>189</v>
+        <v>125</v>
       </c>
       <c r="E93" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F93" t="n">
         <v>0</v>
@@ -11041,10 +11041,10 @@
         <v>669</v>
       </c>
       <c r="D94" t="n">
-        <v>228</v>
+        <v>148</v>
       </c>
       <c r="E94" t="n">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="F94" t="n">
         <v>0</v>
@@ -11172,10 +11172,10 @@
         <v>659</v>
       </c>
       <c r="D95" t="n">
-        <v>254</v>
+        <v>168</v>
       </c>
       <c r="E95" t="n">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="F95" t="n">
         <v>0</v>
@@ -11303,10 +11303,10 @@
         <v>788</v>
       </c>
       <c r="D96" t="n">
-        <v>272</v>
+        <v>189</v>
       </c>
       <c r="E96" t="n">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="F96" t="n">
         <v>0</v>
@@ -11440,10 +11440,10 @@
         <v>681</v>
       </c>
       <c r="D97" t="n">
-        <v>297</v>
+        <v>228</v>
       </c>
       <c r="E97" t="n">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="F97" t="n">
         <v>0</v>
@@ -11577,10 +11577,10 @@
         <v>480</v>
       </c>
       <c r="D98" t="n">
-        <v>332</v>
+        <v>254</v>
       </c>
       <c r="E98" t="n">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="F98" t="n">
         <v>0</v>
@@ -11714,10 +11714,10 @@
         <v>988</v>
       </c>
       <c r="D99" t="n">
-        <v>361</v>
+        <v>272</v>
       </c>
       <c r="E99" t="n">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="F99" t="n">
         <v>0</v>
@@ -11851,10 +11851,10 @@
         <v>1092</v>
       </c>
       <c r="D100" t="n">
-        <v>396</v>
+        <v>297</v>
       </c>
       <c r="E100" t="n">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="F100" t="n">
         <v>0</v>
@@ -11988,7 +11988,7 @@
         <v>877</v>
       </c>
       <c r="D101" t="n">
-        <v>431</v>
+        <v>332</v>
       </c>
       <c r="E101" t="n">
         <v>35</v>
@@ -12125,10 +12125,10 @@
         <v>1441</v>
       </c>
       <c r="D102" t="n">
-        <v>463</v>
+        <v>361</v>
       </c>
       <c r="E102" t="n">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F102" t="n">
         <v>0</v>
@@ -12262,7 +12262,7 @@
         <v>890</v>
       </c>
       <c r="D103" t="n">
-        <v>498</v>
+        <v>396</v>
       </c>
       <c r="E103" t="n">
         <v>35</v>
@@ -12399,10 +12399,10 @@
         <v>923</v>
       </c>
       <c r="D104" t="n">
-        <v>535</v>
+        <v>431</v>
       </c>
       <c r="E104" t="n">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F104" t="n">
         <v>0</v>
@@ -12548,7 +12548,7 @@
         <v>422</v>
       </c>
       <c r="D105" t="n">
-        <v>567</v>
+        <v>463</v>
       </c>
       <c r="E105" t="n">
         <v>32</v>
@@ -12697,10 +12697,10 @@
         <v>718</v>
       </c>
       <c r="D106" t="n">
-        <v>605</v>
+        <v>498</v>
       </c>
       <c r="E106" t="n">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F106" t="n">
         <v>0</v>
@@ -12846,10 +12846,10 @@
         <v>868</v>
       </c>
       <c r="D107" t="n">
-        <v>634</v>
+        <v>535</v>
       </c>
       <c r="E107" t="n">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="F107" t="n">
         <v>0</v>
@@ -12995,10 +12995,10 @@
         <v>963</v>
       </c>
       <c r="D108" t="n">
-        <v>663</v>
+        <v>567</v>
       </c>
       <c r="E108" t="n">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="F108" t="n">
         <v>0</v>
@@ -13144,10 +13144,10 @@
         <v>916</v>
       </c>
       <c r="D109" t="n">
-        <v>690</v>
+        <v>605</v>
       </c>
       <c r="E109" t="n">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="F109" t="n">
         <v>0</v>
@@ -13293,10 +13293,10 @@
         <v>889</v>
       </c>
       <c r="D110" t="n">
-        <v>731</v>
+        <v>634</v>
       </c>
       <c r="E110" t="n">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="F110" t="n">
         <v>0</v>
@@ -13442,10 +13442,10 @@
         <v>663</v>
       </c>
       <c r="D111" t="n">
-        <v>762</v>
+        <v>663</v>
       </c>
       <c r="E111" t="n">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F111" t="n">
         <v>0</v>
@@ -13591,10 +13591,10 @@
         <v>535</v>
       </c>
       <c r="D112" t="n">
-        <v>801</v>
+        <v>690</v>
       </c>
       <c r="E112" t="n">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="F112" t="n">
         <v>0</v>
@@ -13740,10 +13740,10 @@
         <v>738</v>
       </c>
       <c r="D113" t="n">
-        <v>834</v>
+        <v>731</v>
       </c>
       <c r="E113" t="n">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="F113" t="n">
         <v>159732</v>
@@ -13889,10 +13889,10 @@
         <v>873</v>
       </c>
       <c r="D114" t="n">
-        <v>871</v>
+        <v>762</v>
       </c>
       <c r="E114" t="n">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="F114" t="n">
         <v>166291</v>
@@ -14038,10 +14038,10 @@
         <v>875</v>
       </c>
       <c r="D115" t="n">
-        <v>902</v>
+        <v>801</v>
       </c>
       <c r="E115" t="n">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="F115" t="n">
         <v>168259</v>
@@ -14187,10 +14187,10 @@
         <v>862</v>
       </c>
       <c r="D116" t="n">
-        <v>929</v>
+        <v>834</v>
       </c>
       <c r="E116" t="n">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="F116" t="n">
         <v>192594</v>
@@ -14336,10 +14336,10 @@
         <v>967</v>
       </c>
       <c r="D117" t="n">
-        <v>965</v>
+        <v>871</v>
       </c>
       <c r="E117" t="n">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F117" t="n">
         <v>207176</v>
@@ -14485,10 +14485,10 @@
         <v>858</v>
       </c>
       <c r="D118" t="n">
-        <v>990</v>
+        <v>902</v>
       </c>
       <c r="E118" t="n">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="F118" t="n">
         <v>209808</v>
@@ -14634,10 +14634,10 @@
         <v>666</v>
       </c>
       <c r="D119" t="n">
-        <v>1026</v>
+        <v>929</v>
       </c>
       <c r="E119" t="n">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="F119" t="n">
         <v>218668</v>
@@ -14783,10 +14783,10 @@
         <v>874</v>
       </c>
       <c r="D120" t="n">
-        <v>1070</v>
+        <v>965</v>
       </c>
       <c r="E120" t="n">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="F120" t="n">
         <v>222037</v>
@@ -14932,10 +14932,10 @@
         <v>883</v>
       </c>
       <c r="D121" t="n">
-        <v>1103</v>
+        <v>990</v>
       </c>
       <c r="E121" t="n">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="F121" t="n">
         <v>236697</v>
@@ -15081,10 +15081,10 @@
         <v>1033</v>
       </c>
       <c r="D122" t="n">
-        <v>1140</v>
+        <v>1026</v>
       </c>
       <c r="E122" t="n">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F122" t="n">
         <v>247200</v>
@@ -15230,10 +15230,10 @@
         <v>1142</v>
       </c>
       <c r="D123" t="n">
-        <v>1171</v>
+        <v>1070</v>
       </c>
       <c r="E123" t="n">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="F123" t="n">
         <v>246567</v>
@@ -15379,10 +15379,10 @@
         <v>1293</v>
       </c>
       <c r="D124" t="n">
-        <v>1201</v>
+        <v>1103</v>
       </c>
       <c r="E124" t="n">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="F124" t="n">
         <v>257306</v>
@@ -15528,10 +15528,10 @@
         <v>1026</v>
       </c>
       <c r="D125" t="n">
-        <v>1234</v>
+        <v>1140</v>
       </c>
       <c r="E125" t="n">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="F125" t="n">
         <v>257977</v>
@@ -15677,10 +15677,10 @@
         <v>784</v>
       </c>
       <c r="D126" t="n">
-        <v>1271</v>
+        <v>1171</v>
       </c>
       <c r="E126" t="n">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="F126" t="n">
         <v>272725</v>
@@ -15826,10 +15826,10 @@
         <v>1037</v>
       </c>
       <c r="D127" t="n">
-        <v>1305</v>
+        <v>1201</v>
       </c>
       <c r="E127" t="n">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F127" t="n">
         <v>0</v>
@@ -15975,10 +15975,10 @@
         <v>1053</v>
       </c>
       <c r="D128" t="n">
-        <v>1333</v>
+        <v>1234</v>
       </c>
       <c r="E128" t="n">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="F128" t="n">
         <v>292037</v>
@@ -16124,10 +16124,10 @@
         <v>968</v>
       </c>
       <c r="D129" t="n">
-        <v>1361</v>
+        <v>1271</v>
       </c>
       <c r="E129" t="n">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="F129" t="n">
         <v>314439</v>
@@ -16273,10 +16273,10 @@
         <v>1219</v>
       </c>
       <c r="D130" t="n">
-        <v>1397</v>
+        <v>1305</v>
       </c>
       <c r="E130" t="n">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F130" t="n">
         <v>341218</v>
@@ -16422,10 +16422,10 @@
         <v>1251</v>
       </c>
       <c r="D131" t="n">
-        <v>1431</v>
+        <v>1333</v>
       </c>
       <c r="E131" t="n">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="F131" t="n">
         <v>363188</v>
@@ -16575,10 +16575,10 @@
         <v>1009</v>
       </c>
       <c r="D132" t="n">
-        <v>1474</v>
+        <v>1361</v>
       </c>
       <c r="E132" t="n">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="F132" t="n">
         <v>387227</v>
@@ -16728,10 +16728,10 @@
         <v>1000</v>
       </c>
       <c r="D133" t="n">
-        <v>1505</v>
+        <v>1397</v>
       </c>
       <c r="E133" t="n">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="F133" t="n">
         <v>407026</v>
@@ -16881,10 +16881,10 @@
         <v>1179</v>
       </c>
       <c r="D134" t="n">
-        <v>1549</v>
+        <v>1431</v>
       </c>
       <c r="E134" t="n">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="F134" t="n">
         <v>440063</v>
@@ -17034,10 +17034,10 @@
         <v>1355</v>
       </c>
       <c r="D135" t="n">
-        <v>1580</v>
+        <v>1474</v>
       </c>
       <c r="E135" t="n">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="F135" t="n">
         <v>459530</v>
@@ -17187,10 +17187,10 @@
         <v>1448</v>
       </c>
       <c r="D136" t="n">
-        <v>1607</v>
+        <v>1505</v>
       </c>
       <c r="E136" t="n">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="F136" t="n">
         <v>488426</v>
@@ -17340,10 +17340,10 @@
         <v>1347</v>
       </c>
       <c r="D137" t="n">
-        <v>1629</v>
+        <v>1549</v>
       </c>
       <c r="E137" t="n">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="F137" t="n">
         <v>494909</v>
@@ -17509,10 +17509,10 @@
         <v>1801</v>
       </c>
       <c r="D138" t="n">
-        <v>1659</v>
+        <v>1580</v>
       </c>
       <c r="E138" t="n">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F138" t="n">
         <v>514435</v>
@@ -17684,10 +17684,10 @@
         <v>785</v>
       </c>
       <c r="D139" t="n">
-        <v>1681</v>
+        <v>1607</v>
       </c>
       <c r="E139" t="n">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="F139" t="n">
         <v>538559</v>
@@ -17859,10 +17859,10 @@
         <v>909</v>
       </c>
       <c r="D140" t="n">
-        <v>1707</v>
+        <v>1629</v>
       </c>
       <c r="E140" t="n">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F140" t="n">
         <v>567282</v>
@@ -18034,10 +18034,10 @@
         <v>1219</v>
       </c>
       <c r="D141" t="n">
-        <v>1736</v>
+        <v>1659</v>
       </c>
       <c r="E141" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F141" t="n">
         <v>600816</v>
@@ -18209,10 +18209,10 @@
         <v>1411</v>
       </c>
       <c r="D142" t="n">
-        <v>1751</v>
+        <v>1681</v>
       </c>
       <c r="E142" t="n">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="F142" t="n">
         <v>624101</v>
@@ -18384,10 +18384,10 @@
         <v>945</v>
       </c>
       <c r="D143" t="n">
-        <v>1785</v>
+        <v>1707</v>
       </c>
       <c r="E143" t="n">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="F143" t="n">
         <v>643274</v>
@@ -18559,10 +18559,10 @@
         <v>1181</v>
       </c>
       <c r="D144" t="n">
-        <v>1816</v>
+        <v>1736</v>
       </c>
       <c r="E144" t="n">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F144" t="n">
         <v>660292</v>
@@ -18734,10 +18734,10 @@
         <v>1060</v>
       </c>
       <c r="D145" t="n">
-        <v>1839</v>
+        <v>1751</v>
       </c>
       <c r="E145" t="n">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="F145" t="n">
         <v>0</v>
@@ -18899,10 +18899,10 @@
         <v>839</v>
       </c>
       <c r="D146" t="n">
-        <v>1862</v>
+        <v>1785</v>
       </c>
       <c r="E146" t="n">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="F146" t="n">
         <v>693081</v>
@@ -19074,10 +19074,10 @@
         <v>623</v>
       </c>
       <c r="D147" t="n">
-        <v>1894</v>
+        <v>1816</v>
       </c>
       <c r="E147" t="n">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F147" t="n">
         <v>715555</v>
@@ -19249,10 +19249,10 @@
         <v>589</v>
       </c>
       <c r="D148" t="n">
-        <v>1930</v>
+        <v>1839</v>
       </c>
       <c r="E148" t="n">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="F148" t="n">
         <v>735081</v>
@@ -19424,10 +19424,10 @@
         <v>1361</v>
       </c>
       <c r="D149" t="n">
-        <v>1961</v>
+        <v>1862</v>
       </c>
       <c r="E149" t="n">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="F149" t="n">
         <v>749249</v>
@@ -19599,10 +19599,10 @@
         <v>1855</v>
       </c>
       <c r="D150" t="n">
-        <v>1975</v>
+        <v>1894</v>
       </c>
       <c r="E150" t="n">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="F150" t="n">
         <v>773877</v>
@@ -19774,10 +19774,10 @@
         <v>1230</v>
       </c>
       <c r="D151" t="n">
-        <v>1996</v>
+        <v>1930</v>
       </c>
       <c r="E151" t="n">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="F151" t="n">
         <v>790564</v>
@@ -19949,10 +19949,10 @@
         <v>1332</v>
       </c>
       <c r="D152" t="n">
-        <v>2024</v>
+        <v>1961</v>
       </c>
       <c r="E152" t="n">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="F152" t="n">
         <v>813397</v>
@@ -20118,10 +20118,10 @@
         <v>1949</v>
       </c>
       <c r="D153" t="n">
-        <v>2056</v>
+        <v>1975</v>
       </c>
       <c r="E153" t="n">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="F153" t="n">
         <v>820912</v>
@@ -20293,10 +20293,10 @@
         <v>593</v>
       </c>
       <c r="D154" t="n">
-        <v>2078</v>
+        <v>1996</v>
       </c>
       <c r="E154" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F154" t="n">
         <v>865155</v>
@@ -20470,10 +20470,10 @@
         <v>1688</v>
       </c>
       <c r="D155" t="n">
-        <v>2104</v>
+        <v>2024</v>
       </c>
       <c r="E155" t="n">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F155" t="n">
         <v>903048</v>
@@ -20647,10 +20647,10 @@
         <v>1703</v>
       </c>
       <c r="D156" t="n">
-        <v>2137</v>
+        <v>2056</v>
       </c>
       <c r="E156" t="n">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F156" t="n">
         <v>899228</v>
@@ -20824,10 +20824,10 @@
         <v>1649</v>
       </c>
       <c r="D157" t="n">
-        <v>2157</v>
+        <v>2078</v>
       </c>
       <c r="E157" t="n">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F157" t="n">
         <v>923236</v>
@@ -21001,10 +21001,10 @@
         <v>1693</v>
       </c>
       <c r="D158" t="n">
-        <v>2188</v>
+        <v>2104</v>
       </c>
       <c r="E158" t="n">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="F158" t="n">
         <v>935487</v>
@@ -21178,10 +21178,10 @@
         <v>1940</v>
       </c>
       <c r="D159" t="n">
-        <v>2222</v>
+        <v>2137</v>
       </c>
       <c r="E159" t="n">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F159" t="n">
         <v>960363</v>
@@ -21355,10 +21355,10 @@
         <v>1425</v>
       </c>
       <c r="D160" t="n">
-        <v>2246</v>
+        <v>2157</v>
       </c>
       <c r="E160" t="n">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F160" t="n">
         <v>1014824</v>
@@ -21532,10 +21532,10 @@
         <v>638</v>
       </c>
       <c r="D161" t="n">
-        <v>2274</v>
+        <v>2188</v>
       </c>
       <c r="E161" t="n">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="F161" t="n">
         <v>1029197</v>
@@ -21709,10 +21709,10 @@
         <v>1637</v>
       </c>
       <c r="D162" t="n">
-        <v>2309</v>
+        <v>2222</v>
       </c>
       <c r="E162" t="n">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F162" t="n">
         <v>1051218</v>
@@ -21886,10 +21886,10 @@
         <v>2504</v>
       </c>
       <c r="D163" t="n">
-        <v>2349</v>
+        <v>2246</v>
       </c>
       <c r="E163" t="n">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="F163" t="n">
         <v>0</v>
@@ -22063,10 +22063,10 @@
         <v>1826</v>
       </c>
       <c r="D164" t="n">
-        <v>2395</v>
+        <v>2274</v>
       </c>
       <c r="E164" t="n">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="F164" t="n">
         <v>1070849</v>
@@ -22240,10 +22240,10 @@
         <v>2097</v>
       </c>
       <c r="D165" t="n">
-        <v>2424</v>
+        <v>2309</v>
       </c>
       <c r="E165" t="n">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="F165" t="n">
         <v>1072466</v>
@@ -22417,10 +22417,10 @@
         <v>2331</v>
       </c>
       <c r="D166" t="n">
-        <v>2469</v>
+        <v>2349</v>
       </c>
       <c r="E166" t="n">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="F166" t="n">
         <v>1088326</v>
@@ -22594,10 +22594,10 @@
         <v>1843</v>
       </c>
       <c r="D167" t="n">
-        <v>2506</v>
+        <v>2395</v>
       </c>
       <c r="E167" t="n">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="F167" t="n">
         <v>1112677</v>
@@ -22771,10 +22771,10 @@
         <v>1254</v>
       </c>
       <c r="D168" t="n">
-        <v>2548</v>
+        <v>2424</v>
       </c>
       <c r="E168" t="n">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="F168" t="n">
         <v>1135749</v>
@@ -22948,10 +22948,10 @@
         <v>4098</v>
       </c>
       <c r="D169" t="n">
-        <v>2594</v>
+        <v>2469</v>
       </c>
       <c r="E169" t="n">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F169" t="n">
         <v>1169385</v>
@@ -23125,10 +23125,10 @@
         <v>3129</v>
       </c>
       <c r="D170" t="n">
-        <v>2641</v>
+        <v>2506</v>
       </c>
       <c r="E170" t="n">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="F170" t="n">
         <v>1187367</v>
@@ -23302,10 +23302,10 @@
         <v>3516</v>
       </c>
       <c r="D171" t="n">
-        <v>2681</v>
+        <v>2548</v>
       </c>
       <c r="E171" t="n">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="F171" t="n">
         <v>1212302</v>
@@ -23479,10 +23479,10 @@
         <v>3454</v>
       </c>
       <c r="D172" t="n">
-        <v>2724</v>
+        <v>2594</v>
       </c>
       <c r="E172" t="n">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="F172" t="n">
         <v>1249858</v>
@@ -23656,10 +23656,10 @@
         <v>4430</v>
       </c>
       <c r="D173" t="n">
-        <v>2765</v>
+        <v>2641</v>
       </c>
       <c r="E173" t="n">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="F173" t="n">
         <v>1286735</v>
@@ -23833,10 +23833,10 @@
         <v>3866</v>
       </c>
       <c r="D174" t="n">
-        <v>2837</v>
+        <v>2681</v>
       </c>
       <c r="E174" t="n">
-        <v>72</v>
+        <v>40</v>
       </c>
       <c r="F174" t="n">
         <v>1313265</v>
@@ -24010,10 +24010,10 @@
         <v>3280</v>
       </c>
       <c r="D175" t="n">
-        <v>2895</v>
+        <v>2724</v>
       </c>
       <c r="E175" t="n">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="F175" t="n">
         <v>1350920</v>
@@ -24187,10 +24187,10 @@
         <v>5489</v>
       </c>
       <c r="D176" t="n">
-        <v>2961</v>
+        <v>2765</v>
       </c>
       <c r="E176" t="n">
-        <v>66</v>
+        <v>41</v>
       </c>
       <c r="F176" t="n">
         <v>0</v>
@@ -24364,10 +24364,10 @@
         <v>5551</v>
       </c>
       <c r="D177" t="n">
-        <v>3037</v>
+        <v>2837</v>
       </c>
       <c r="E177" t="n">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F177" t="n">
         <v>1399304</v>
@@ -24541,10 +24541,10 @@
         <v>5996</v>
       </c>
       <c r="D178" t="n">
-        <v>3124</v>
+        <v>2895</v>
       </c>
       <c r="E178" t="n">
-        <v>87</v>
+        <v>58</v>
       </c>
       <c r="F178" t="n">
         <v>1409858</v>
@@ -24718,10 +24718,10 @@
         <v>5707</v>
       </c>
       <c r="D179" t="n">
-        <v>3209</v>
+        <v>2961</v>
       </c>
       <c r="E179" t="n">
-        <v>85</v>
+        <v>66</v>
       </c>
       <c r="F179" t="n">
         <v>1444189</v>
@@ -24895,10 +24895,10 @@
         <v>5742</v>
       </c>
       <c r="D180" t="n">
-        <v>3291</v>
+        <v>3037</v>
       </c>
       <c r="E180" t="n">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="F180" t="n">
         <v>1492340</v>
@@ -25072,10 +25072,10 @@
         <v>5357</v>
       </c>
       <c r="D181" t="n">
-        <v>3380</v>
+        <v>3124</v>
       </c>
       <c r="E181" t="n">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F181" t="n">
         <v>1543186</v>
@@ -25249,10 +25249,10 @@
         <v>4288</v>
       </c>
       <c r="D182" t="n">
-        <v>3482</v>
+        <v>3209</v>
       </c>
       <c r="E182" t="n">
-        <v>102</v>
+        <v>85</v>
       </c>
       <c r="F182" t="n">
         <v>1578667</v>
@@ -25426,10 +25426,10 @@
         <v>6975</v>
       </c>
       <c r="D183" t="n">
-        <v>3600</v>
+        <v>3291</v>
       </c>
       <c r="E183" t="n">
-        <v>118</v>
+        <v>82</v>
       </c>
       <c r="F183" t="n">
         <v>1612583</v>
@@ -25603,10 +25603,10 @@
         <v>8076</v>
       </c>
       <c r="D184" t="n">
-        <v>3727</v>
+        <v>3380</v>
       </c>
       <c r="E184" t="n">
-        <v>127</v>
+        <v>89</v>
       </c>
       <c r="F184" t="n">
         <v>1653835</v>
@@ -25782,10 +25782,10 @@
         <v>7915</v>
       </c>
       <c r="D185" t="n">
-        <v>3837</v>
+        <v>3482</v>
       </c>
       <c r="E185" t="n">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="F185" t="n">
         <v>1696809</v>
@@ -25961,10 +25961,10 @@
         <v>7555</v>
       </c>
       <c r="D186" t="n">
-        <v>3951</v>
+        <v>3600</v>
       </c>
       <c r="E186" t="n">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="F186" t="n">
         <v>1741722</v>
@@ -26140,10 +26140,10 @@
         <v>8258</v>
       </c>
       <c r="D187" t="n">
-        <v>4083</v>
+        <v>3727</v>
       </c>
       <c r="E187" t="n">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="F187" t="n">
         <v>1785542</v>
@@ -26319,10 +26319,10 @@
         <v>3449</v>
       </c>
       <c r="D188" t="n">
-        <v>4227</v>
+        <v>3837</v>
       </c>
       <c r="E188" t="n">
-        <v>144</v>
+        <v>110</v>
       </c>
       <c r="F188" t="n">
         <v>1829966</v>
@@ -26498,10 +26498,10 @@
         <v>5318</v>
       </c>
       <c r="D189" t="n">
-        <v>4359</v>
+        <v>3951</v>
       </c>
       <c r="E189" t="n">
-        <v>132</v>
+        <v>114</v>
       </c>
       <c r="F189" t="n">
         <v>1874626</v>
@@ -26677,10 +26677,10 @@
         <v>10028</v>
       </c>
       <c r="D190" t="n">
-        <v>4504</v>
+        <v>4083</v>
       </c>
       <c r="E190" t="n">
-        <v>145</v>
+        <v>132</v>
       </c>
       <c r="F190" t="n">
         <v>1917116</v>
@@ -26856,10 +26856,10 @@
         <v>9979</v>
       </c>
       <c r="D191" t="n">
-        <v>4641</v>
+        <v>4227</v>
       </c>
       <c r="E191" t="n">
-        <v>137</v>
+        <v>144</v>
       </c>
       <c r="F191" t="n">
         <v>1960005</v>
@@ -27035,10 +27035,10 @@
         <v>9782</v>
       </c>
       <c r="D192" t="n">
-        <v>4810</v>
+        <v>4359</v>
       </c>
       <c r="E192" t="n">
-        <v>169</v>
+        <v>132</v>
       </c>
       <c r="F192" t="n">
         <v>2020405</v>
@@ -27214,10 +27214,10 @@
         <v>9765</v>
       </c>
       <c r="D193" t="n">
-        <v>4946</v>
+        <v>4504</v>
       </c>
       <c r="E193" t="n">
-        <v>136</v>
+        <v>145</v>
       </c>
       <c r="F193" t="n">
         <v>2069122</v>
@@ -27393,10 +27393,10 @@
         <v>10351</v>
       </c>
       <c r="D194" t="n">
-        <v>5101</v>
+        <v>4641</v>
       </c>
       <c r="E194" t="n">
-        <v>155</v>
+        <v>137</v>
       </c>
       <c r="F194" t="n">
         <v>2110922</v>
@@ -27572,10 +27572,10 @@
         <v>8196</v>
       </c>
       <c r="D195" t="n">
-        <v>5232</v>
+        <v>4810</v>
       </c>
       <c r="E195" t="n">
-        <v>131</v>
+        <v>169</v>
       </c>
       <c r="F195" t="n">
         <v>2165623</v>
@@ -27751,10 +27751,10 @@
         <v>5655</v>
       </c>
       <c r="D196" t="n">
-        <v>5338</v>
+        <v>4946</v>
       </c>
       <c r="E196" t="n">
-        <v>106</v>
+        <v>136</v>
       </c>
       <c r="F196" t="n">
         <v>2205822</v>
@@ -27930,10 +27930,10 @@
         <v>10745</v>
       </c>
       <c r="D197" t="n">
-        <v>5432</v>
+        <v>5101</v>
       </c>
       <c r="E197" t="n">
-        <v>94</v>
+        <v>155</v>
       </c>
       <c r="F197" t="n">
         <v>2249060</v>
@@ -28109,10 +28109,10 @@
         <v>7307</v>
       </c>
       <c r="D198" t="n">
-        <v>5509</v>
+        <v>5232</v>
       </c>
       <c r="E198" t="n">
-        <v>77</v>
+        <v>131</v>
       </c>
       <c r="F198" t="n">
         <v>2286774</v>
@@ -28252,10 +28252,10 @@
         <v>10291</v>
       </c>
       <c r="D199" t="n">
-        <v>5580</v>
+        <v>5338</v>
       </c>
       <c r="E199" t="n">
-        <v>71</v>
+        <v>106</v>
       </c>
       <c r="F199" t="n">
         <v>2301483</v>
@@ -28395,10 +28395,10 @@
         <v>14916</v>
       </c>
       <c r="D200" t="n">
-        <v>5642</v>
+        <v>5432</v>
       </c>
       <c r="E200" t="n">
-        <v>62</v>
+        <v>94</v>
       </c>
       <c r="F200" t="n">
         <v>2343210</v>
@@ -28538,10 +28538,10 @@
         <v>10158</v>
       </c>
       <c r="D201" t="n">
-        <v>5679</v>
+        <v>5509</v>
       </c>
       <c r="E201" t="n">
-        <v>37</v>
+        <v>77</v>
       </c>
       <c r="F201" t="n">
         <v>2384232</v>
@@ -28681,10 +28681,10 @@
         <v>7300</v>
       </c>
       <c r="D202" t="n">
-        <v>5705</v>
+        <v>5580</v>
       </c>
       <c r="E202" t="n">
-        <v>26</v>
+        <v>71</v>
       </c>
       <c r="F202" t="n">
         <v>2439082</v>
@@ -28824,10 +28824,10 @@
         <v>7404</v>
       </c>
       <c r="D203" t="n">
-        <v>5710</v>
+        <v>5642</v>
       </c>
       <c r="E203" t="n">
-        <v>5</v>
+        <v>62</v>
       </c>
       <c r="F203" t="n">
         <v>2473836</v>
@@ -28967,10 +28967,10 @@
         <v>9305</v>
       </c>
       <c r="D204" t="n">
-        <v>5711</v>
+        <v>5679</v>
       </c>
       <c r="E204" t="n">
-        <v>1</v>
+        <v>37</v>
       </c>
       <c r="F204" t="n">
         <v>2514877</v>
@@ -29094,10 +29094,10 @@
         <v>9879</v>
       </c>
       <c r="D205" t="n">
-        <v>0</v>
+        <v>5705</v>
       </c>
       <c r="E205" t="n">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="F205" t="n">
         <v>2544071</v>
@@ -29219,15 +29219,9 @@
       <c r="BC205"/>
       <c r="BD205"/>
       <c r="BE205"/>
-      <c r="BF205" t="n">
-        <v>415</v>
-      </c>
-      <c r="BG205" t="n">
-        <v>482</v>
-      </c>
-      <c r="BH205" t="n">
-        <v>86.1</v>
-      </c>
+      <c r="BF205"/>
+      <c r="BG205"/>
+      <c r="BH205"/>
       <c r="BI205" t="n">
         <v>29677668</v>
       </c>
@@ -29243,10 +29237,10 @@
         <v>9507</v>
       </c>
       <c r="D206" t="n">
-        <v>0</v>
+        <v>5710</v>
       </c>
       <c r="E206" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F206" t="n">
         <v>2574376</v>
@@ -29386,10 +29380,10 @@
         <v>8701</v>
       </c>
       <c r="D207" t="n">
-        <v>0</v>
+        <v>5711</v>
       </c>
       <c r="E207" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F207" t="n">
         <v>2609056</v>
@@ -29682,10 +29676,10 @@
         <v>38531</v>
       </c>
       <c r="H209" t="n">
-        <v>161705</v>
+        <v>163376</v>
       </c>
       <c r="I209" t="n">
-        <v>0</v>
+        <v>1671</v>
       </c>
       <c r="J209" t="e">
         <v>#NUM!</v>
@@ -29924,10 +29918,153 @@
       <c r="BC210"/>
       <c r="BD210"/>
       <c r="BE210"/>
-      <c r="BF210"/>
-      <c r="BG210"/>
-      <c r="BH210"/>
+      <c r="BF210" t="n">
+        <v>415</v>
+      </c>
+      <c r="BG210" t="n">
+        <v>482</v>
+      </c>
+      <c r="BH210" t="n">
+        <v>86.1</v>
+      </c>
       <c r="BI210" t="n">
+        <v>29677668</v>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" s="1" t="n">
+        <v>44039</v>
+      </c>
+      <c r="B211" t="n">
+        <v>385924</v>
+      </c>
+      <c r="C211" t="n">
+        <v>4268</v>
+      </c>
+      <c r="D211" t="n">
+        <v>0</v>
+      </c>
+      <c r="E211" t="n">
+        <v>0</v>
+      </c>
+      <c r="F211" t="n">
+        <v>0</v>
+      </c>
+      <c r="G211" t="n">
+        <v>0</v>
+      </c>
+      <c r="H211" t="n">
+        <v>0</v>
+      </c>
+      <c r="I211" t="n">
+        <v>0</v>
+      </c>
+      <c r="J211" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="K211" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="L211" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="M211" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="N211" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="O211" t="e">
+        <v>#NUM!</v>
+      </c>
+      <c r="P211"/>
+      <c r="Q211"/>
+      <c r="R211" t="n">
+        <v>3714821</v>
+      </c>
+      <c r="S211"/>
+      <c r="T211"/>
+      <c r="U211"/>
+      <c r="V211"/>
+      <c r="W211" t="n">
+        <v>9781</v>
+      </c>
+      <c r="X211" t="n">
+        <v>480</v>
+      </c>
+      <c r="Y211" t="n">
+        <v>1694</v>
+      </c>
+      <c r="Z211" t="n">
+        <v>255</v>
+      </c>
+      <c r="AA211" t="n">
+        <v>568</v>
+      </c>
+      <c r="AB211" t="n">
+        <v>937</v>
+      </c>
+      <c r="AC211" t="n">
+        <v>14485</v>
+      </c>
+      <c r="AD211" t="n">
+        <v>1894</v>
+      </c>
+      <c r="AE211" t="n">
+        <v>5257</v>
+      </c>
+      <c r="AF211" t="n">
+        <v>6965</v>
+      </c>
+      <c r="AG211" t="n">
+        <v>5574</v>
+      </c>
+      <c r="AH211" t="n">
+        <v>3088</v>
+      </c>
+      <c r="AI211" t="n">
+        <v>15026</v>
+      </c>
+      <c r="AJ211" t="n">
+        <v>2233</v>
+      </c>
+      <c r="AK211" t="n">
+        <v>22703</v>
+      </c>
+      <c r="AL211" t="n">
+        <v>6989</v>
+      </c>
+      <c r="AM211" t="n">
+        <v>6073</v>
+      </c>
+      <c r="AN211"/>
+      <c r="AO211"/>
+      <c r="AP211"/>
+      <c r="AQ211"/>
+      <c r="AR211"/>
+      <c r="AS211"/>
+      <c r="AT211"/>
+      <c r="AU211"/>
+      <c r="AV211"/>
+      <c r="AW211"/>
+      <c r="AX211"/>
+      <c r="AY211"/>
+      <c r="AZ211"/>
+      <c r="BA211"/>
+      <c r="BB211"/>
+      <c r="BC211"/>
+      <c r="BD211"/>
+      <c r="BE211"/>
+      <c r="BF211" t="n">
+        <v>467</v>
+      </c>
+      <c r="BG211" t="n">
+        <v>507</v>
+      </c>
+      <c r="BH211" t="n">
+        <v>92.11</v>
+      </c>
+      <c r="BI211" t="n">
         <v>29677668</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update files to match new changes
</commit_message>
<xml_diff>
--- a/combined-datasets/state.xlsx
+++ b/combined-datasets/state.xlsx
@@ -7629,7 +7629,7 @@
         <v>43897</v>
       </c>
       <c r="B68" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C68" t="n">
         <v>0</v>
@@ -7760,7 +7760,7 @@
         <v>43898</v>
       </c>
       <c r="B69" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C69" t="n">
         <v>0</v>
@@ -8546,7 +8546,7 @@
         <v>43904</v>
       </c>
       <c r="B75" t="n">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="C75" t="n">
         <v>0</v>
@@ -15832,7 +15832,7 @@
         <v>30</v>
       </c>
       <c r="F127" t="n">
-        <v>0</v>
+        <v>272725</v>
       </c>
       <c r="G127" t="n">
         <v>0</v>
@@ -15984,7 +15984,7 @@
         <v>292037</v>
       </c>
       <c r="G128" t="n">
-        <v>0</v>
+        <v>19312</v>
       </c>
       <c r="H128" t="n">
         <v>19318</v>
@@ -18740,7 +18740,7 @@
         <v>15</v>
       </c>
       <c r="F145" t="n">
-        <v>0</v>
+        <v>660292</v>
       </c>
       <c r="G145" t="n">
         <v>0</v>
@@ -18908,7 +18908,7 @@
         <v>693081</v>
       </c>
       <c r="G146" t="n">
-        <v>0</v>
+        <v>32789</v>
       </c>
       <c r="H146" t="n">
         <v>27045</v>
@@ -21892,7 +21892,7 @@
         <v>24</v>
       </c>
       <c r="F163" t="n">
-        <v>0</v>
+        <v>1051218</v>
       </c>
       <c r="G163" t="n">
         <v>0</v>
@@ -22072,7 +22072,7 @@
         <v>1070849</v>
       </c>
       <c r="G164" t="n">
-        <v>0</v>
+        <v>19631</v>
       </c>
       <c r="H164" t="n">
         <v>33639</v>
@@ -24193,7 +24193,7 @@
         <v>41</v>
       </c>
       <c r="F176" t="n">
-        <v>0</v>
+        <v>1350920</v>
       </c>
       <c r="G176" t="n">
         <v>0</v>
@@ -29523,7 +29523,7 @@
         <v>6020</v>
       </c>
       <c r="D208" t="n">
-        <v>0</v>
+        <v>5711</v>
       </c>
       <c r="E208" t="n">
         <v>0</v>
@@ -29664,7 +29664,7 @@
         <v>5810</v>
       </c>
       <c r="D209" t="n">
-        <v>0</v>
+        <v>5711</v>
       </c>
       <c r="E209" t="n">
         <v>0</v>
@@ -29805,19 +29805,19 @@
         <v>4268</v>
       </c>
       <c r="D210" t="n">
-        <v>0</v>
+        <v>5711</v>
       </c>
       <c r="E210" t="n">
         <v>0</v>
       </c>
       <c r="F210" t="n">
-        <v>0</v>
+        <v>2676478</v>
       </c>
       <c r="G210" t="n">
         <v>0</v>
       </c>
       <c r="H210" t="n">
-        <v>0</v>
+        <v>163376</v>
       </c>
       <c r="I210" t="n">
         <v>0</v>
@@ -29942,19 +29942,19 @@
         <v>4268</v>
       </c>
       <c r="D211" t="n">
-        <v>0</v>
+        <v>5711</v>
       </c>
       <c r="E211" t="n">
         <v>0</v>
       </c>
       <c r="F211" t="n">
-        <v>0</v>
+        <v>2676478</v>
       </c>
       <c r="G211" t="n">
         <v>0</v>
       </c>
       <c r="H211" t="n">
-        <v>0</v>
+        <v>163376</v>
       </c>
       <c r="I211" t="n">
         <v>0</v>
@@ -30068,6 +30068,89 @@
         <v>29677668</v>
       </c>
     </row>
+    <row r="212">
+      <c r="A212" s="1" t="n">
+        <v>44040</v>
+      </c>
+      <c r="B212"/>
+      <c r="C212"/>
+      <c r="D212"/>
+      <c r="E212"/>
+      <c r="F212"/>
+      <c r="G212"/>
+      <c r="H212"/>
+      <c r="I212"/>
+      <c r="J212"/>
+      <c r="K212"/>
+      <c r="L212"/>
+      <c r="M212"/>
+      <c r="N212"/>
+      <c r="O212"/>
+      <c r="P212"/>
+      <c r="Q212"/>
+      <c r="R212"/>
+      <c r="S212"/>
+      <c r="T212"/>
+      <c r="U212"/>
+      <c r="V212"/>
+      <c r="W212"/>
+      <c r="X212" t="n">
+        <v>484</v>
+      </c>
+      <c r="Y212" t="n">
+        <v>1791</v>
+      </c>
+      <c r="Z212" t="n">
+        <v>265</v>
+      </c>
+      <c r="AA212" t="n">
+        <v>600</v>
+      </c>
+      <c r="AB212" t="n">
+        <v>941</v>
+      </c>
+      <c r="AC212" t="n">
+        <v>14867</v>
+      </c>
+      <c r="AD212" t="n">
+        <v>1973</v>
+      </c>
+      <c r="AE212" t="n">
+        <v>5544</v>
+      </c>
+      <c r="AF212"/>
+      <c r="AG212"/>
+      <c r="AH212"/>
+      <c r="AI212"/>
+      <c r="AJ212"/>
+      <c r="AK212"/>
+      <c r="AL212"/>
+      <c r="AM212"/>
+      <c r="AN212"/>
+      <c r="AO212"/>
+      <c r="AP212"/>
+      <c r="AQ212"/>
+      <c r="AR212"/>
+      <c r="AS212"/>
+      <c r="AT212"/>
+      <c r="AU212"/>
+      <c r="AV212"/>
+      <c r="AW212"/>
+      <c r="AX212"/>
+      <c r="AY212"/>
+      <c r="AZ212"/>
+      <c r="BA212"/>
+      <c r="BB212"/>
+      <c r="BC212"/>
+      <c r="BD212"/>
+      <c r="BE212"/>
+      <c r="BF212"/>
+      <c r="BG212"/>
+      <c r="BH212"/>
+      <c r="BI212" t="n">
+        <v>29677668</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>

<commit_message>
fix hospital factor handling
</commit_message>
<xml_diff>
--- a/combined-datasets/state.xlsx
+++ b/combined-datasets/state.xlsx
@@ -4856,22 +4856,16 @@
         <v>1338</v>
       </c>
       <c r="AF41">
-        <v>229</v>
+        <v>1338</v>
       </c>
       <c r="AG41">
-        <v>189</v>
+        <v>775</v>
       </c>
       <c r="AH41">
-        <v>182</v>
-      </c>
-      <c r="AI41">
-        <v>247</v>
-      </c>
-      <c r="AJ41">
-        <v>237</v>
+        <v>563</v>
       </c>
       <c r="AK41">
-        <v>253</v>
+        <v>27420</v>
       </c>
       <c r="AN41">
         <v>29035.98470826723</v>
@@ -4987,22 +4981,16 @@
         <v>1176</v>
       </c>
       <c r="AF42">
-        <v>439</v>
+        <v>1176</v>
       </c>
       <c r="AG42">
-        <v>358</v>
+        <v>585</v>
       </c>
       <c r="AH42">
-        <v>308</v>
-      </c>
-      <c r="AI42">
-        <v>638</v>
-      </c>
-      <c r="AJ42">
-        <v>472</v>
+        <v>591</v>
       </c>
       <c r="AK42">
-        <v>700</v>
+        <v>26721</v>
       </c>
       <c r="AN42">
         <v>28825.46103115658</v>
@@ -5118,22 +5106,16 @@
         <v>1409</v>
       </c>
       <c r="AF43">
-        <v>547</v>
+        <v>1409</v>
       </c>
       <c r="AG43">
-        <v>413</v>
+        <v>815</v>
       </c>
       <c r="AH43">
-        <v>359</v>
-      </c>
-      <c r="AI43">
-        <v>988</v>
-      </c>
-      <c r="AJ43">
-        <v>809</v>
+        <v>594</v>
       </c>
       <c r="AK43">
-        <v>1199</v>
+        <v>28695</v>
       </c>
       <c r="AN43">
         <v>31752.6202178227</v>
@@ -5249,22 +5231,16 @@
         <v>1538</v>
       </c>
       <c r="AF44">
-        <v>581</v>
+        <v>1568</v>
       </c>
       <c r="AG44">
-        <v>442</v>
+        <v>880</v>
       </c>
       <c r="AH44">
-        <v>387</v>
-      </c>
-      <c r="AI44">
-        <v>1291</v>
-      </c>
-      <c r="AJ44">
-        <v>834</v>
+        <v>688</v>
       </c>
       <c r="AK44">
-        <v>1479</v>
+        <v>29892</v>
       </c>
       <c r="AN44">
         <v>31813.96100657447</v>
@@ -5380,22 +5356,16 @@
         <v>1459</v>
       </c>
       <c r="AF45">
-        <v>570</v>
+        <v>1459</v>
       </c>
       <c r="AG45">
-        <v>472</v>
+        <v>796</v>
       </c>
       <c r="AH45">
-        <v>448</v>
-      </c>
-      <c r="AI45">
-        <v>1656</v>
-      </c>
-      <c r="AJ45">
-        <v>976</v>
+        <v>663</v>
       </c>
       <c r="AK45">
-        <v>1889</v>
+        <v>30271</v>
       </c>
       <c r="AN45">
         <v>32902.65852646294</v>
@@ -5511,22 +5481,16 @@
         <v>1522</v>
       </c>
       <c r="AF46">
-        <v>673</v>
+        <v>1522</v>
       </c>
       <c r="AG46">
-        <v>571</v>
+        <v>828</v>
       </c>
       <c r="AH46">
-        <v>442</v>
-      </c>
-      <c r="AI46">
-        <v>1937</v>
-      </c>
-      <c r="AJ46">
-        <v>996</v>
+        <v>694</v>
       </c>
       <c r="AK46">
-        <v>2217</v>
+        <v>30162</v>
       </c>
       <c r="AN46">
         <v>33022.9761352849</v>
@@ -5642,22 +5606,16 @@
         <v>1321</v>
       </c>
       <c r="AF47">
-        <v>827</v>
+        <v>1321</v>
       </c>
       <c r="AG47">
-        <v>523</v>
+        <v>738</v>
       </c>
       <c r="AH47">
-        <v>405</v>
-      </c>
-      <c r="AI47">
-        <v>2441</v>
-      </c>
-      <c r="AJ47">
-        <v>1164</v>
+        <v>583</v>
       </c>
       <c r="AK47">
-        <v>2455</v>
+        <v>30333</v>
       </c>
       <c r="AN47">
         <v>32155.1932118547</v>
@@ -5773,22 +5731,16 @@
         <v>1471</v>
       </c>
       <c r="AF48">
-        <v>704</v>
+        <v>1471</v>
       </c>
       <c r="AG48">
-        <v>515</v>
+        <v>847</v>
       </c>
       <c r="AH48">
-        <v>383</v>
-      </c>
-      <c r="AI48">
-        <v>2790</v>
-      </c>
-      <c r="AJ48">
-        <v>1257</v>
+        <v>624</v>
       </c>
       <c r="AK48">
-        <v>3008</v>
+        <v>29136</v>
       </c>
       <c r="AN48">
         <v>31120.76245246267</v>
@@ -5904,22 +5856,16 @@
         <v>1411</v>
       </c>
       <c r="AF49">
-        <v>739</v>
+        <v>1414</v>
       </c>
       <c r="AG49">
-        <v>559</v>
+        <v>794</v>
       </c>
       <c r="AH49">
-        <v>491</v>
-      </c>
-      <c r="AI49">
-        <v>2908</v>
-      </c>
-      <c r="AJ49">
-        <v>1242</v>
+        <v>620</v>
       </c>
       <c r="AK49">
-        <v>3691</v>
+        <v>27057</v>
       </c>
       <c r="AN49">
         <v>32267.95564097237</v>
@@ -6035,22 +5981,16 @@
         <v>1419</v>
       </c>
       <c r="AF50">
-        <v>916</v>
+        <v>1497</v>
       </c>
       <c r="AG50">
-        <v>666</v>
+        <v>861</v>
       </c>
       <c r="AH50">
-        <v>541</v>
-      </c>
-      <c r="AI50">
-        <v>3305</v>
-      </c>
-      <c r="AJ50">
-        <v>971</v>
+        <v>636</v>
       </c>
       <c r="AK50">
-        <v>3909</v>
+        <v>29380</v>
       </c>
       <c r="AN50">
         <v>34405.61838918673</v>
@@ -6166,22 +6106,16 @@
         <v>1678</v>
       </c>
       <c r="AF51">
-        <v>1117</v>
+        <v>1678</v>
       </c>
       <c r="AG51">
-        <v>749</v>
+        <v>987</v>
       </c>
       <c r="AH51">
-        <v>612</v>
-      </c>
-      <c r="AI51">
-        <v>3687</v>
-      </c>
-      <c r="AJ51">
-        <v>1190</v>
+        <v>691</v>
       </c>
       <c r="AK51">
-        <v>4356</v>
+        <v>32474</v>
       </c>
       <c r="AN51">
         <v>34727.73740020218</v>
@@ -6297,22 +6231,16 @@
         <v>1649</v>
       </c>
       <c r="AF52">
-        <v>1129</v>
+        <v>1649</v>
       </c>
       <c r="AG52">
-        <v>557</v>
+        <v>960</v>
       </c>
       <c r="AH52">
-        <v>652</v>
-      </c>
-      <c r="AI52">
-        <v>4076</v>
-      </c>
-      <c r="AJ52">
-        <v>1356</v>
+        <v>689</v>
       </c>
       <c r="AK52">
-        <v>4145</v>
+        <v>34032</v>
       </c>
       <c r="AN52">
         <v>34790.47844708776</v>
@@ -6428,22 +6356,16 @@
         <v>1674</v>
       </c>
       <c r="AF53">
-        <v>1092</v>
+        <v>1664</v>
       </c>
       <c r="AG53">
-        <v>675</v>
+        <v>994</v>
       </c>
       <c r="AH53">
-        <v>520</v>
-      </c>
-      <c r="AI53">
-        <v>3810</v>
-      </c>
-      <c r="AJ53">
-        <v>1758</v>
+        <v>670</v>
       </c>
       <c r="AK53">
-        <v>4705</v>
+        <v>34788</v>
       </c>
       <c r="AN53">
         <v>35467.93083732159</v>
@@ -6559,22 +6481,16 @@
         <v>1597</v>
       </c>
       <c r="AF54">
-        <v>1110</v>
+        <v>1587</v>
       </c>
       <c r="AG54">
-        <v>736</v>
+        <v>946</v>
       </c>
       <c r="AH54">
-        <v>566</v>
-      </c>
-      <c r="AI54">
-        <v>3542</v>
-      </c>
-      <c r="AJ54">
-        <v>1281</v>
+        <v>651</v>
       </c>
       <c r="AK54">
-        <v>4787</v>
+        <v>34687</v>
       </c>
       <c r="AN54">
         <v>33774.36982228375</v>
@@ -6690,22 +6606,16 @@
         <v>1542</v>
       </c>
       <c r="AF55">
-        <v>1076</v>
+        <v>1542</v>
       </c>
       <c r="AG55">
-        <v>647</v>
+        <v>897</v>
       </c>
       <c r="AH55">
-        <v>567</v>
-      </c>
-      <c r="AI55">
-        <v>4386</v>
-      </c>
-      <c r="AJ55">
-        <v>1409</v>
+        <v>645</v>
       </c>
       <c r="AK55">
-        <v>5091</v>
+        <v>33201</v>
       </c>
       <c r="AN55">
         <v>33154.08506676356</v>
@@ -6821,22 +6731,16 @@
         <v>1563</v>
       </c>
       <c r="AF56">
-        <v>1172</v>
+        <v>1563</v>
       </c>
       <c r="AG56">
-        <v>644</v>
+        <v>903</v>
       </c>
       <c r="AH56">
-        <v>578</v>
-      </c>
-      <c r="AI56">
-        <v>4789</v>
-      </c>
-      <c r="AJ56">
-        <v>1579</v>
+        <v>660</v>
       </c>
       <c r="AK56">
-        <v>4700</v>
+        <v>31702</v>
       </c>
       <c r="AN56">
         <v>33843.43827408803</v>
@@ -6952,22 +6856,16 @@
         <v>1682</v>
       </c>
       <c r="AF57">
-        <v>1129</v>
+        <v>1682</v>
       </c>
       <c r="AG57">
-        <v>721</v>
+        <v>998</v>
       </c>
       <c r="AH57">
-        <v>490</v>
-      </c>
-      <c r="AI57">
-        <v>5614</v>
-      </c>
-      <c r="AJ57">
-        <v>1382</v>
+        <v>684</v>
       </c>
       <c r="AK57">
-        <v>5805</v>
+        <v>33473</v>
       </c>
       <c r="AN57">
         <v>35746.9254658385</v>
@@ -7083,22 +6981,16 @@
         <v>1702</v>
       </c>
       <c r="AF58">
-        <v>1278</v>
+        <v>1702</v>
       </c>
       <c r="AG58">
-        <v>655</v>
+        <v>984</v>
       </c>
       <c r="AH58">
-        <v>667</v>
-      </c>
-      <c r="AI58">
-        <v>4831</v>
-      </c>
-      <c r="AJ58">
-        <v>1750</v>
+        <v>718</v>
       </c>
       <c r="AK58">
-        <v>6501</v>
+        <v>35289</v>
       </c>
       <c r="AN58">
         <v>36408.60414932941</v>
@@ -7214,22 +7106,16 @@
         <v>1686</v>
       </c>
       <c r="AF59">
-        <v>1150</v>
+        <v>1686</v>
       </c>
       <c r="AG59">
-        <v>877</v>
+        <v>982</v>
       </c>
       <c r="AH59">
-        <v>552</v>
-      </c>
-      <c r="AI59">
-        <v>5182</v>
-      </c>
-      <c r="AJ59">
-        <v>1382</v>
+        <v>704</v>
       </c>
       <c r="AK59">
-        <v>6771</v>
+        <v>35604</v>
       </c>
       <c r="AN59">
         <v>36360.70649995992</v>
@@ -7345,22 +7231,16 @@
         <v>1778</v>
       </c>
       <c r="AF60">
-        <v>1283</v>
+        <v>1778</v>
       </c>
       <c r="AG60">
-        <v>609</v>
+        <v>1042</v>
       </c>
       <c r="AH60">
-        <v>549</v>
-      </c>
-      <c r="AI60">
-        <v>5335</v>
-      </c>
-      <c r="AJ60">
-        <v>2007</v>
+        <v>736</v>
       </c>
       <c r="AK60">
-        <v>7178</v>
+        <v>36409</v>
       </c>
       <c r="AN60">
         <v>35631.30094526693</v>
@@ -7476,22 +7356,16 @@
         <v>1725</v>
       </c>
       <c r="AF61">
-        <v>1091</v>
+        <v>1725</v>
       </c>
       <c r="AG61">
-        <v>853</v>
+        <v>1014</v>
       </c>
       <c r="AH61">
-        <v>684</v>
-      </c>
-      <c r="AI61">
-        <v>5521</v>
-      </c>
-      <c r="AJ61">
-        <v>1689</v>
+        <v>711</v>
       </c>
       <c r="AK61">
-        <v>6955</v>
+        <v>35692</v>
       </c>
       <c r="AN61">
         <v>34916.65057895484</v>
@@ -7607,22 +7481,16 @@
         <v>1540</v>
       </c>
       <c r="AF62">
-        <v>1125</v>
+        <v>1540</v>
       </c>
       <c r="AG62">
-        <v>958</v>
+        <v>916</v>
       </c>
       <c r="AH62">
-        <v>546</v>
-      </c>
-      <c r="AI62">
-        <v>5977</v>
-      </c>
-      <c r="AJ62">
-        <v>1548</v>
+        <v>624</v>
       </c>
       <c r="AK62">
-        <v>6400</v>
+        <v>32012</v>
       </c>
       <c r="AN62">
         <v>34225.37768214206</v>
@@ -7738,22 +7606,16 @@
         <v>1533</v>
       </c>
       <c r="AF63">
-        <v>1114</v>
+        <v>1533</v>
       </c>
       <c r="AG63">
-        <v>750</v>
+        <v>914</v>
       </c>
       <c r="AH63">
-        <v>572</v>
-      </c>
-      <c r="AI63">
-        <v>6021</v>
-      </c>
-      <c r="AJ63">
-        <v>1505</v>
+        <v>619</v>
       </c>
       <c r="AK63">
-        <v>7057</v>
+        <v>32019</v>
       </c>
       <c r="AN63">
         <v>35433.20080251558</v>
@@ -7869,22 +7731,16 @@
         <v>1888</v>
       </c>
       <c r="AF64">
-        <v>1258</v>
+        <v>1888</v>
       </c>
       <c r="AG64">
-        <v>707</v>
+        <v>1199</v>
       </c>
       <c r="AH64">
-        <v>556</v>
-      </c>
-      <c r="AI64">
-        <v>5631</v>
-      </c>
-      <c r="AJ64">
-        <v>1947</v>
+        <v>689</v>
       </c>
       <c r="AK64">
-        <v>7607</v>
+        <v>34653</v>
       </c>
       <c r="AN64">
         <v>37685.83486469234</v>
@@ -8000,22 +7856,16 @@
         <v>1812</v>
       </c>
       <c r="AF65">
-        <v>1322</v>
+        <v>1812</v>
       </c>
       <c r="AG65">
-        <v>1020</v>
+        <v>1086</v>
       </c>
       <c r="AH65">
-        <v>658</v>
-      </c>
-      <c r="AI65">
-        <v>7204</v>
-      </c>
-      <c r="AJ65">
-        <v>1688</v>
+        <v>726</v>
       </c>
       <c r="AK65">
-        <v>7879</v>
+        <v>37421</v>
       </c>
       <c r="AN65">
         <v>38789.7745921801</v>
@@ -8131,22 +7981,16 @@
         <v>1750</v>
       </c>
       <c r="AF66">
-        <v>1089</v>
+        <v>1750</v>
       </c>
       <c r="AG66">
-        <v>784</v>
+        <v>1034</v>
       </c>
       <c r="AH66">
-        <v>634</v>
-      </c>
-      <c r="AI66">
-        <v>6952</v>
-      </c>
-      <c r="AJ66">
-        <v>1800</v>
+        <v>716</v>
       </c>
       <c r="AK66">
-        <v>8886</v>
+        <v>38722</v>
       </c>
       <c r="AN66">
         <v>38425.01917592684</v>
@@ -8262,22 +8106,16 @@
         <v>1734</v>
       </c>
       <c r="AF67">
-        <v>1327</v>
+        <v>1734</v>
       </c>
       <c r="AG67">
-        <v>851</v>
+        <v>1037</v>
       </c>
       <c r="AH67">
-        <v>649</v>
-      </c>
-      <c r="AI67">
-        <v>6611</v>
-      </c>
-      <c r="AJ67">
-        <v>1940</v>
+        <v>697</v>
       </c>
       <c r="AK67">
-        <v>8982</v>
+        <v>38516</v>
       </c>
       <c r="AN67">
         <v>37904.79560820685</v>
@@ -8399,22 +8237,16 @@
         <v>1735</v>
       </c>
       <c r="AF68">
-        <v>1623</v>
+        <v>1735</v>
       </c>
       <c r="AG68">
-        <v>975</v>
+        <v>1061</v>
       </c>
       <c r="AH68">
-        <v>537</v>
-      </c>
-      <c r="AI68">
-        <v>6992</v>
-      </c>
-      <c r="AJ68">
-        <v>1768</v>
+        <v>674</v>
       </c>
       <c r="AK68">
-        <v>8593</v>
+        <v>37977</v>
       </c>
       <c r="AN68">
         <v>36082.18332613036</v>
@@ -8536,22 +8368,16 @@
         <v>1626</v>
       </c>
       <c r="AF69">
-        <v>1333</v>
+        <v>1626</v>
       </c>
       <c r="AG69">
-        <v>888</v>
+        <v>965</v>
       </c>
       <c r="AH69">
-        <v>560</v>
-      </c>
-      <c r="AI69">
-        <v>6987</v>
-      </c>
-      <c r="AJ69">
-        <v>1795</v>
+        <v>661</v>
       </c>
       <c r="AK69">
-        <v>7667</v>
+        <v>35333</v>
       </c>
       <c r="AN69">
         <v>34567.59939467562</v>
@@ -8673,22 +8499,16 @@
         <v>1525</v>
       </c>
       <c r="AF70">
-        <v>1256</v>
+        <v>1525</v>
       </c>
       <c r="AG70">
-        <v>890</v>
+        <v>915</v>
       </c>
       <c r="AH70">
-        <v>515</v>
-      </c>
-      <c r="AI70">
-        <v>7179</v>
-      </c>
-      <c r="AJ70">
-        <v>1393</v>
+        <v>610</v>
       </c>
       <c r="AK70">
-        <v>7984</v>
+        <v>32549</v>
       </c>
       <c r="AN70">
         <v>35910.12239490647</v>
@@ -8810,22 +8630,16 @@
         <v>1725</v>
       </c>
       <c r="AF71">
-        <v>1303</v>
+        <v>1725</v>
       </c>
       <c r="AG71">
-        <v>954</v>
+        <v>1026</v>
       </c>
       <c r="AH71">
-        <v>654</v>
-      </c>
-      <c r="AI71">
-        <v>7293</v>
-      </c>
-      <c r="AJ71">
-        <v>1278</v>
+        <v>699</v>
       </c>
       <c r="AK71">
-        <v>8896</v>
+        <v>34519</v>
       </c>
       <c r="AN71">
         <v>37795.2508037951</v>
@@ -8947,22 +8761,16 @@
         <v>1676</v>
       </c>
       <c r="AF72">
-        <v>1410</v>
+        <v>1676</v>
       </c>
       <c r="AG72">
-        <v>914</v>
+        <v>1002</v>
       </c>
       <c r="AH72">
-        <v>616</v>
-      </c>
-      <c r="AI72">
-        <v>7568</v>
-      </c>
-      <c r="AJ72">
-        <v>1799</v>
+        <v>674</v>
       </c>
       <c r="AK72">
-        <v>10658</v>
+        <v>38292</v>
       </c>
       <c r="AN72">
         <v>38947.37170394264</v>
@@ -9084,22 +8892,16 @@
         <v>1648</v>
       </c>
       <c r="AF73">
-        <v>1056</v>
+        <v>1648</v>
       </c>
       <c r="AG73">
-        <v>1018</v>
+        <v>975</v>
       </c>
       <c r="AH73">
-        <v>614</v>
-      </c>
-      <c r="AI73">
-        <v>7695</v>
-      </c>
-      <c r="AJ73">
-        <v>2062</v>
+        <v>673</v>
       </c>
       <c r="AK73">
-        <v>9833</v>
+        <v>38626</v>
       </c>
       <c r="AN73">
         <v>39385.60682618964</v>
@@ -9245,22 +9047,16 @@
         <v>494</v>
       </c>
       <c r="AF74">
-        <v>1550</v>
+        <v>1716</v>
       </c>
       <c r="AG74">
-        <v>1053</v>
+        <v>1033</v>
       </c>
       <c r="AH74">
-        <v>706</v>
-      </c>
-      <c r="AI74">
-        <v>8067</v>
-      </c>
-      <c r="AJ74">
-        <v>1959</v>
+        <v>683</v>
       </c>
       <c r="AK74">
-        <v>8352</v>
+        <v>39654</v>
       </c>
       <c r="AN74">
         <v>39049.043149967</v>
@@ -9415,22 +9211,16 @@
         <v>530</v>
       </c>
       <c r="AF75">
-        <v>1245</v>
+        <v>1791</v>
       </c>
       <c r="AG75">
-        <v>974</v>
+        <v>1104</v>
       </c>
       <c r="AH75">
-        <v>662</v>
-      </c>
-      <c r="AI75">
-        <v>7500</v>
-      </c>
-      <c r="AJ75">
-        <v>2123</v>
+        <v>687</v>
       </c>
       <c r="AK75">
-        <v>10382</v>
+        <v>39392</v>
       </c>
       <c r="AN75">
         <v>36487.94347595329</v>
@@ -9585,22 +9375,16 @@
         <v>531</v>
       </c>
       <c r="AF76">
-        <v>1392</v>
+        <v>1512</v>
       </c>
       <c r="AG76">
-        <v>886</v>
+        <v>908</v>
       </c>
       <c r="AH76">
-        <v>520</v>
-      </c>
-      <c r="AI76">
-        <v>9004</v>
-      </c>
-      <c r="AJ76">
-        <v>2340</v>
+        <v>604</v>
       </c>
       <c r="AK76">
-        <v>9405</v>
+        <v>34208</v>
       </c>
       <c r="AN76">
         <v>35651.80314401623</v>
@@ -9755,22 +9539,16 @@
         <v>575</v>
       </c>
       <c r="AF77">
-        <v>1219</v>
+        <v>1551</v>
       </c>
       <c r="AG77">
-        <v>847</v>
+        <v>933</v>
       </c>
       <c r="AH77">
-        <v>517</v>
-      </c>
-      <c r="AI77">
-        <v>9120</v>
-      </c>
-      <c r="AJ77">
-        <v>2322</v>
+        <v>618</v>
       </c>
       <c r="AK77">
-        <v>9902</v>
+        <v>33455</v>
       </c>
       <c r="AN77">
         <v>37230.45407108596</v>
@@ -9925,22 +9703,16 @@
         <v>631</v>
       </c>
       <c r="AF78">
-        <v>1353</v>
+        <v>1732</v>
       </c>
       <c r="AG78">
-        <v>1064</v>
+        <v>1057</v>
       </c>
       <c r="AH78">
-        <v>542</v>
-      </c>
-      <c r="AI78">
-        <v>7597</v>
-      </c>
-      <c r="AJ78">
-        <v>1802</v>
+        <v>675</v>
       </c>
       <c r="AK78">
-        <v>11703</v>
+        <v>35767</v>
       </c>
       <c r="AN78">
         <v>40050.25805684386</v>
@@ -10095,22 +9867,16 @@
         <v>684</v>
       </c>
       <c r="AF79">
-        <v>1613</v>
+        <v>1791</v>
       </c>
       <c r="AG79">
-        <v>1307</v>
+        <v>1097</v>
       </c>
       <c r="AH79">
-        <v>663</v>
-      </c>
-      <c r="AI79">
-        <v>8348</v>
-      </c>
-      <c r="AJ79">
-        <v>1738</v>
+        <v>694</v>
       </c>
       <c r="AK79">
-        <v>10815</v>
+        <v>40313</v>
       </c>
       <c r="AN79">
         <v>41497.40748947485</v>
@@ -10265,22 +10031,16 @@
         <v>719</v>
       </c>
       <c r="AF80">
-        <v>1510</v>
+        <v>1680</v>
       </c>
       <c r="AG80">
-        <v>998</v>
+        <v>990</v>
       </c>
       <c r="AH80">
-        <v>655</v>
-      </c>
-      <c r="AI80">
-        <v>9018</v>
-      </c>
-      <c r="AJ80">
-        <v>2111</v>
+        <v>690</v>
       </c>
       <c r="AK80">
-        <v>12773</v>
+        <v>40321</v>
       </c>
       <c r="AN80">
         <v>41292.61982144648</v>
@@ -10435,22 +10195,16 @@
         <v>730</v>
       </c>
       <c r="AF81">
-        <v>1446</v>
+        <v>1578</v>
       </c>
       <c r="AG81">
-        <v>860</v>
+        <v>913</v>
       </c>
       <c r="AH81">
-        <v>587</v>
-      </c>
-      <c r="AI81">
-        <v>8725</v>
-      </c>
-      <c r="AJ81">
-        <v>2469</v>
+        <v>665</v>
       </c>
       <c r="AK81">
-        <v>11710</v>
+        <v>40132</v>
       </c>
       <c r="AN81">
         <v>40674.18455489584</v>
@@ -10590,22 +10344,16 @@
         <v>800</v>
       </c>
       <c r="AF82">
-        <v>1472</v>
+        <v>1688</v>
       </c>
       <c r="AG82">
-        <v>1123</v>
+        <v>1022</v>
       </c>
       <c r="AH82">
-        <v>521</v>
-      </c>
-      <c r="AI82">
-        <v>9150</v>
-      </c>
-      <c r="AJ82">
-        <v>2189</v>
+        <v>666</v>
       </c>
       <c r="AK82">
-        <v>13032</v>
+        <v>40977</v>
       </c>
       <c r="AN82">
         <v>39147.50616003113</v>
@@ -10760,22 +10508,16 @@
         <v>812</v>
       </c>
       <c r="AF83">
-        <v>1652</v>
+        <v>1572</v>
       </c>
       <c r="AG83">
-        <v>927</v>
+        <v>929</v>
       </c>
       <c r="AH83">
-        <v>639</v>
-      </c>
-      <c r="AI83">
-        <v>9702</v>
-      </c>
-      <c r="AJ83">
-        <v>1603</v>
+        <v>643</v>
       </c>
       <c r="AK83">
-        <v>11813</v>
+        <v>35987</v>
       </c>
       <c r="AN83">
         <v>37612.64530774832</v>
@@ -10930,22 +10672,16 @@
         <v>885</v>
       </c>
       <c r="AF84">
-        <v>1285</v>
+        <v>1511</v>
       </c>
       <c r="AG84">
-        <v>1072</v>
+        <v>854</v>
       </c>
       <c r="AH84">
-        <v>544</v>
-      </c>
-      <c r="AI84">
-        <v>9172</v>
-      </c>
-      <c r="AJ84">
-        <v>1931</v>
+        <v>657</v>
       </c>
       <c r="AK84">
-        <v>11316</v>
+        <v>33489</v>
       </c>
       <c r="AN84">
         <v>37863.02706368687</v>
@@ -11100,22 +10836,16 @@
         <v>940</v>
       </c>
       <c r="AF85">
-        <v>1253</v>
+        <v>1534</v>
       </c>
       <c r="AG85">
-        <v>992</v>
+        <v>887</v>
       </c>
       <c r="AH85">
-        <v>711</v>
-      </c>
-      <c r="AI85">
-        <v>8372</v>
-      </c>
-      <c r="AJ85">
-        <v>2212</v>
+        <v>647</v>
       </c>
       <c r="AK85">
-        <v>13556</v>
+        <v>34246</v>
       </c>
       <c r="AN85">
         <v>38886.3669035533</v>
@@ -11270,22 +11000,16 @@
         <v>982</v>
       </c>
       <c r="AF86">
-        <v>1295</v>
+        <v>1645</v>
       </c>
       <c r="AG86">
-        <v>873</v>
+        <v>974</v>
       </c>
       <c r="AH86">
-        <v>594</v>
-      </c>
-      <c r="AI86">
-        <v>7783</v>
-      </c>
-      <c r="AJ86">
-        <v>2088</v>
+        <v>671</v>
       </c>
       <c r="AK86">
-        <v>12457</v>
+        <v>36501</v>
       </c>
       <c r="AN86">
         <v>41229.61555479576</v>
@@ -11440,22 +11164,16 @@
         <v>996</v>
       </c>
       <c r="AF87">
-        <v>1497</v>
+        <v>1692</v>
       </c>
       <c r="AG87">
-        <v>838</v>
+        <v>998</v>
       </c>
       <c r="AH87">
-        <v>660</v>
-      </c>
-      <c r="AI87">
-        <v>9249</v>
-      </c>
-      <c r="AJ87">
-        <v>2163</v>
+        <v>694</v>
       </c>
       <c r="AK87">
-        <v>13386</v>
+        <v>39561</v>
       </c>
       <c r="AN87">
         <v>41951.73687016795</v>
@@ -11610,22 +11328,22 @@
         <v>1074</v>
       </c>
       <c r="AF88">
-        <v>1525</v>
+        <v>1622</v>
       </c>
       <c r="AG88">
-        <v>823</v>
+        <v>875</v>
       </c>
       <c r="AH88">
-        <v>714</v>
+        <v>747</v>
       </c>
       <c r="AI88">
-        <v>14179</v>
+        <v>16136</v>
       </c>
       <c r="AJ88">
-        <v>5858</v>
+        <v>1696</v>
       </c>
       <c r="AK88">
-        <v>12818</v>
+        <v>41521</v>
       </c>
       <c r="AN88">
         <v>41348.15712741879</v>
@@ -11771,22 +11489,22 @@
         <v>1155</v>
       </c>
       <c r="AF89">
-        <v>1671</v>
+        <v>1752</v>
       </c>
       <c r="AG89">
-        <v>1078</v>
+        <v>999</v>
       </c>
       <c r="AH89">
-        <v>592</v>
+        <v>753</v>
       </c>
       <c r="AI89">
-        <v>14623</v>
+        <v>15599</v>
       </c>
       <c r="AJ89">
-        <v>6102</v>
+        <v>1697</v>
       </c>
       <c r="AK89">
-        <v>11075</v>
+        <v>41462</v>
       </c>
       <c r="AN89">
         <v>39328.28048149107</v>
@@ -11941,22 +11659,22 @@
         <v>1169</v>
       </c>
       <c r="AF90">
-        <v>1540</v>
+        <v>1684</v>
       </c>
       <c r="AG90">
-        <v>945</v>
+        <v>953</v>
       </c>
       <c r="AH90">
-        <v>820</v>
+        <v>731</v>
       </c>
       <c r="AI90">
-        <v>15018</v>
+        <v>16127</v>
       </c>
       <c r="AJ90">
-        <v>6295</v>
+        <v>1698</v>
       </c>
       <c r="AK90">
-        <v>14796</v>
+        <v>39467</v>
       </c>
       <c r="AN90">
         <v>38190.0334571706</v>
@@ -12111,22 +11829,22 @@
         <v>1181</v>
       </c>
       <c r="AF91">
-        <v>1302</v>
+        <v>1756</v>
       </c>
       <c r="AG91">
-        <v>1091</v>
+        <v>1008</v>
       </c>
       <c r="AH91">
-        <v>687</v>
+        <v>748</v>
       </c>
       <c r="AI91">
-        <v>15449</v>
+        <v>16330</v>
       </c>
       <c r="AJ91">
-        <v>6516</v>
+        <v>1784</v>
       </c>
       <c r="AK91">
-        <v>13357</v>
+        <v>38032</v>
       </c>
       <c r="AL91">
         <v>5394</v>
@@ -12284,22 +12002,22 @@
         <v>1254</v>
       </c>
       <c r="AF92">
-        <v>1656</v>
+        <v>1773</v>
       </c>
       <c r="AG92">
-        <v>1046</v>
+        <v>1011</v>
       </c>
       <c r="AH92">
-        <v>689</v>
+        <v>762</v>
       </c>
       <c r="AI92">
-        <v>15773</v>
+        <v>16575</v>
       </c>
       <c r="AJ92">
-        <v>6601</v>
+        <v>1764</v>
       </c>
       <c r="AK92">
-        <v>13409</v>
+        <v>37510</v>
       </c>
       <c r="AL92">
         <v>5314</v>
@@ -12457,22 +12175,22 @@
         <v>1284</v>
       </c>
       <c r="AF93">
-        <v>1230</v>
+        <v>1805</v>
       </c>
       <c r="AG93">
-        <v>1124</v>
+        <v>1057</v>
       </c>
       <c r="AH93">
-        <v>653</v>
+        <v>748</v>
       </c>
       <c r="AI93">
-        <v>16168</v>
+        <v>14948</v>
       </c>
       <c r="AJ93">
-        <v>6465</v>
+        <v>1621</v>
       </c>
       <c r="AK93">
-        <v>13209</v>
+        <v>36201</v>
       </c>
       <c r="AL93">
         <v>5566</v>
@@ -12630,22 +12348,22 @@
         <v>1368</v>
       </c>
       <c r="AF94">
-        <v>1401</v>
+        <v>1796</v>
       </c>
       <c r="AG94">
-        <v>1133</v>
+        <v>1066</v>
       </c>
       <c r="AH94">
-        <v>709</v>
+        <v>730</v>
       </c>
       <c r="AI94">
-        <v>16616</v>
+        <v>15219</v>
       </c>
       <c r="AJ94">
-        <v>6777</v>
+        <v>1658</v>
       </c>
       <c r="AK94">
-        <v>11925</v>
+        <v>40783</v>
       </c>
       <c r="AL94">
         <v>5577</v>
@@ -12803,22 +12521,22 @@
         <v>1437</v>
       </c>
       <c r="AF95">
-        <v>1510</v>
+        <v>1855</v>
       </c>
       <c r="AG95">
-        <v>985</v>
+        <v>1113</v>
       </c>
       <c r="AH95">
-        <v>818</v>
+        <v>742</v>
       </c>
       <c r="AI95">
-        <v>17156</v>
+        <v>14674</v>
       </c>
       <c r="AJ95">
-        <v>6431</v>
+        <v>1625</v>
       </c>
       <c r="AK95">
-        <v>14360</v>
+        <v>42965</v>
       </c>
       <c r="AL95">
         <v>5587</v>
@@ -12976,22 +12694,22 @@
         <v>1495</v>
       </c>
       <c r="AF96">
-        <v>1584</v>
+        <v>1822</v>
       </c>
       <c r="AG96">
-        <v>924</v>
+        <v>1085</v>
       </c>
       <c r="AH96">
-        <v>623</v>
+        <v>737</v>
       </c>
       <c r="AI96">
-        <v>17334</v>
+        <v>15198</v>
       </c>
       <c r="AJ96">
-        <v>6653</v>
+        <v>1583</v>
       </c>
       <c r="AK96">
-        <v>14962</v>
+        <v>41603</v>
       </c>
       <c r="AL96">
         <v>5623</v>
@@ -13149,22 +12867,22 @@
         <v>1499</v>
       </c>
       <c r="AF97">
-        <v>1348</v>
+        <v>1878</v>
       </c>
       <c r="AG97">
-        <v>850</v>
+        <v>1115</v>
       </c>
       <c r="AH97">
-        <v>831</v>
+        <v>763</v>
       </c>
       <c r="AI97">
-        <v>17569</v>
+        <v>15942</v>
       </c>
       <c r="AJ97">
-        <v>6836</v>
+        <v>1680</v>
       </c>
       <c r="AK97">
-        <v>15834</v>
+        <v>40237</v>
       </c>
       <c r="AL97">
         <v>5657</v>
@@ -13322,22 +13040,22 @@
         <v>1512</v>
       </c>
       <c r="AF98">
-        <v>1439</v>
+        <v>1935</v>
       </c>
       <c r="AG98">
-        <v>1077</v>
+        <v>1192</v>
       </c>
       <c r="AH98">
-        <v>800</v>
+        <v>743</v>
       </c>
       <c r="AI98">
-        <v>17766</v>
+        <v>15070</v>
       </c>
       <c r="AJ98">
-        <v>6857</v>
+        <v>1619</v>
       </c>
       <c r="AK98">
-        <v>14681</v>
+        <v>37283</v>
       </c>
       <c r="AL98">
         <v>5292</v>
@@ -13495,22 +13213,22 @@
         <v>1636</v>
       </c>
       <c r="AF99">
-        <v>1827</v>
+        <v>2056</v>
       </c>
       <c r="AG99">
-        <v>1211</v>
+        <v>1272</v>
       </c>
       <c r="AH99">
-        <v>789</v>
+        <v>784</v>
       </c>
       <c r="AI99">
-        <v>17900</v>
+        <v>15402</v>
       </c>
       <c r="AJ99">
-        <v>6867</v>
+        <v>1723</v>
       </c>
       <c r="AK99">
-        <v>14496</v>
+        <v>39336</v>
       </c>
       <c r="AL99">
         <v>5500</v>
@@ -13668,22 +13386,22 @@
         <v>1739</v>
       </c>
       <c r="AF100">
-        <v>1335</v>
+        <v>2153</v>
       </c>
       <c r="AG100">
-        <v>977</v>
+        <v>1296</v>
       </c>
       <c r="AH100">
-        <v>861</v>
+        <v>857</v>
       </c>
       <c r="AI100">
-        <v>17945</v>
+        <v>13645</v>
       </c>
       <c r="AJ100">
-        <v>6796</v>
+        <v>1508</v>
       </c>
       <c r="AK100">
-        <v>16310</v>
+        <v>42410</v>
       </c>
       <c r="AL100">
         <v>5622</v>
@@ -13841,22 +13559,22 @@
         <v>1831</v>
       </c>
       <c r="AF101">
-        <v>1533</v>
+        <v>2059</v>
       </c>
       <c r="AG101">
-        <v>1137</v>
+        <v>1250</v>
       </c>
       <c r="AH101">
-        <v>926</v>
+        <v>809</v>
       </c>
       <c r="AI101">
-        <v>18666</v>
+        <v>13271</v>
       </c>
       <c r="AJ101">
-        <v>6785</v>
+        <v>1419</v>
       </c>
       <c r="AK101">
-        <v>15780</v>
+        <v>40724</v>
       </c>
       <c r="AL101">
         <v>5667</v>
@@ -14014,22 +13732,22 @@
         <v>1908</v>
       </c>
       <c r="AF102">
-        <v>1763</v>
+        <v>2166</v>
       </c>
       <c r="AG102">
-        <v>1327</v>
+        <v>1356</v>
       </c>
       <c r="AH102">
-        <v>890</v>
+        <v>810</v>
       </c>
       <c r="AI102">
-        <v>18455</v>
+        <v>14033</v>
       </c>
       <c r="AJ102">
-        <v>6933</v>
+        <v>1494</v>
       </c>
       <c r="AK102">
-        <v>15779</v>
+        <v>42995</v>
       </c>
       <c r="AL102">
         <v>5726</v>
@@ -14187,22 +13905,22 @@
         <v>1939</v>
       </c>
       <c r="AF103">
-        <v>1707</v>
+        <v>2242</v>
       </c>
       <c r="AG103">
-        <v>1126</v>
+        <v>1414</v>
       </c>
       <c r="AH103">
-        <v>802</v>
+        <v>828</v>
       </c>
       <c r="AI103">
-        <v>18677</v>
+        <v>13571</v>
       </c>
       <c r="AJ103">
-        <v>6906</v>
+        <v>1498</v>
       </c>
       <c r="AK103">
-        <v>14989</v>
+        <v>43025</v>
       </c>
       <c r="AL103">
         <v>5710</v>
@@ -14360,22 +14078,22 @@
         <v>1939</v>
       </c>
       <c r="AF104">
-        <v>1653</v>
+        <v>2287</v>
       </c>
       <c r="AG104">
-        <v>1278</v>
+        <v>1470</v>
       </c>
       <c r="AH104">
-        <v>957</v>
+        <v>817</v>
       </c>
       <c r="AI104">
-        <v>18969</v>
+        <v>14660</v>
       </c>
       <c r="AJ104">
-        <v>7116</v>
+        <v>1603</v>
       </c>
       <c r="AK104">
-        <v>15358</v>
+        <v>40548</v>
       </c>
       <c r="AL104">
         <v>5633</v>
@@ -14533,22 +14251,22 @@
         <v>2015</v>
       </c>
       <c r="AF105">
-        <v>1812</v>
+        <v>2326</v>
       </c>
       <c r="AG105">
-        <v>1209</v>
+        <v>1465</v>
       </c>
       <c r="AH105">
-        <v>970</v>
+        <v>861</v>
       </c>
       <c r="AI105">
-        <v>19374</v>
+        <v>14525</v>
       </c>
       <c r="AJ105">
-        <v>6847</v>
+        <v>1626</v>
       </c>
       <c r="AK105">
-        <v>17191</v>
+        <v>36840</v>
       </c>
       <c r="AL105">
         <v>5289</v>
@@ -14706,22 +14424,22 @@
         <v>2141</v>
       </c>
       <c r="AF106">
-        <v>1805</v>
+        <v>2518</v>
       </c>
       <c r="AG106">
-        <v>1494</v>
+        <v>1623</v>
       </c>
       <c r="AH106">
-        <v>1044</v>
+        <v>895</v>
       </c>
       <c r="AI106">
-        <v>18940</v>
+        <v>14993</v>
       </c>
       <c r="AJ106">
-        <v>7015</v>
+        <v>1675</v>
       </c>
       <c r="AK106">
-        <v>15636</v>
+        <v>39851</v>
       </c>
       <c r="AL106">
         <v>5529</v>
@@ -14879,22 +14597,22 @@
         <v>2242</v>
       </c>
       <c r="AF107">
-        <v>2071</v>
+        <v>2793</v>
       </c>
       <c r="AG107">
-        <v>1612</v>
+        <v>1829</v>
       </c>
       <c r="AH107">
-        <v>1099</v>
+        <v>964</v>
       </c>
       <c r="AI107">
-        <v>19602</v>
+        <v>13815</v>
       </c>
       <c r="AJ107">
-        <v>7218</v>
+        <v>1473</v>
       </c>
       <c r="AK107">
-        <v>17830</v>
+        <v>42379</v>
       </c>
       <c r="AL107">
         <v>5782</v>
@@ -15052,22 +14770,22 @@
         <v>2290</v>
       </c>
       <c r="AF108">
-        <v>2372</v>
+        <v>2947</v>
       </c>
       <c r="AG108">
-        <v>1656</v>
+        <v>1937</v>
       </c>
       <c r="AH108">
-        <v>1152</v>
+        <v>1010</v>
       </c>
       <c r="AI108">
-        <v>20029</v>
+        <v>13472</v>
       </c>
       <c r="AJ108">
-        <v>7611</v>
+        <v>1453</v>
       </c>
       <c r="AK108">
-        <v>16941</v>
+        <v>44041</v>
       </c>
       <c r="AL108">
         <v>5856</v>
@@ -15225,22 +14943,22 @@
         <v>2373</v>
       </c>
       <c r="AF109">
-        <v>2220</v>
+        <v>3148</v>
       </c>
       <c r="AG109">
-        <v>1618</v>
+        <v>2060</v>
       </c>
       <c r="AH109">
-        <v>1245</v>
+        <v>1088</v>
       </c>
       <c r="AI109">
-        <v>20501</v>
+        <v>13591</v>
       </c>
       <c r="AJ109">
-        <v>7130</v>
+        <v>1443</v>
       </c>
       <c r="AK109">
-        <v>17648</v>
+        <v>46232</v>
       </c>
       <c r="AL109">
         <v>5841</v>
@@ -15398,22 +15116,22 @@
         <v>2437</v>
       </c>
       <c r="AF110">
-        <v>2408</v>
+        <v>3247</v>
       </c>
       <c r="AG110">
-        <v>1374</v>
+        <v>2134</v>
       </c>
       <c r="AH110">
-        <v>1154</v>
+        <v>1113</v>
       </c>
       <c r="AI110">
-        <v>19559</v>
+        <v>13701</v>
       </c>
       <c r="AJ110">
-        <v>7088</v>
+        <v>1449</v>
       </c>
       <c r="AK110">
-        <v>18195</v>
+        <v>44293</v>
       </c>
       <c r="AL110">
         <v>5807</v>
@@ -15571,22 +15289,22 @@
         <v>2454</v>
       </c>
       <c r="AF111">
-        <v>2361</v>
+        <v>3409</v>
       </c>
       <c r="AG111">
-        <v>1735</v>
+        <v>2266</v>
       </c>
       <c r="AH111">
-        <v>1193</v>
+        <v>1143</v>
       </c>
       <c r="AI111">
-        <v>19071</v>
+        <v>14316</v>
       </c>
       <c r="AJ111">
-        <v>7267</v>
+        <v>1493</v>
       </c>
       <c r="AK111">
-        <v>14326</v>
+        <v>42815</v>
       </c>
       <c r="AL111">
         <v>5701</v>
@@ -15744,22 +15462,22 @@
         <v>2481</v>
       </c>
       <c r="AF112">
-        <v>2358</v>
+        <v>3711</v>
       </c>
       <c r="AG112">
-        <v>1653</v>
+        <v>2491</v>
       </c>
       <c r="AH112">
-        <v>1103</v>
+        <v>1220</v>
       </c>
       <c r="AI112">
-        <v>19828</v>
+        <v>14697</v>
       </c>
       <c r="AJ112">
-        <v>6944</v>
+        <v>1517</v>
       </c>
       <c r="AK112">
-        <v>14832</v>
+        <v>40607</v>
       </c>
       <c r="AL112">
         <v>5712</v>
@@ -15917,22 +15635,22 @@
         <v>2501</v>
       </c>
       <c r="AF113">
-        <v>2336</v>
+        <v>4092</v>
       </c>
       <c r="AG113">
-        <v>1700</v>
+        <v>2767</v>
       </c>
       <c r="AH113">
-        <v>1279</v>
+        <v>1325</v>
       </c>
       <c r="AI113">
-        <v>21289</v>
+        <v>14260</v>
       </c>
       <c r="AJ113">
-        <v>7263</v>
+        <v>1483</v>
       </c>
       <c r="AK113">
-        <v>14540</v>
+        <v>40382</v>
       </c>
       <c r="AL113">
         <v>5762</v>
@@ -16090,22 +15808,22 @@
         <v>2557</v>
       </c>
       <c r="AF114">
-        <v>2762</v>
+        <v>4389</v>
       </c>
       <c r="AG114">
-        <v>1848</v>
+        <v>2990</v>
       </c>
       <c r="AH114">
-        <v>1144</v>
+        <v>1399</v>
       </c>
       <c r="AI114">
-        <v>21266</v>
+        <v>12951</v>
       </c>
       <c r="AJ114">
-        <v>7212</v>
+        <v>1320</v>
       </c>
       <c r="AK114">
-        <v>17380</v>
+        <v>43756</v>
       </c>
       <c r="AL114">
         <v>5968</v>
@@ -16263,22 +15981,22 @@
         <v>2629</v>
       </c>
       <c r="AF115">
-        <v>2615</v>
+        <v>4739</v>
       </c>
       <c r="AG115">
-        <v>2202</v>
+        <v>3279</v>
       </c>
       <c r="AH115">
-        <v>1358</v>
+        <v>1460</v>
       </c>
       <c r="AI115">
-        <v>19872</v>
+        <v>12597</v>
       </c>
       <c r="AJ115">
-        <v>7223</v>
+        <v>1322</v>
       </c>
       <c r="AK115">
-        <v>17819</v>
+        <v>45208</v>
       </c>
       <c r="AL115">
         <v>6051</v>
@@ -16436,22 +16154,22 @@
         <v>2684</v>
       </c>
       <c r="AF116">
-        <v>3150</v>
+        <v>5102</v>
       </c>
       <c r="AG116">
-        <v>1971</v>
+        <v>3516</v>
       </c>
       <c r="AH116">
-        <v>1443</v>
+        <v>1586</v>
       </c>
       <c r="AI116">
-        <v>20575</v>
+        <v>12398</v>
       </c>
       <c r="AJ116">
-        <v>7142</v>
+        <v>1284</v>
       </c>
       <c r="AK116">
-        <v>19436</v>
+        <v>45535</v>
       </c>
       <c r="AL116">
         <v>6150</v>
@@ -16609,22 +16327,22 @@
         <v>2705</v>
       </c>
       <c r="AF117">
-        <v>2918</v>
+        <v>5523</v>
       </c>
       <c r="AG117">
-        <v>2038</v>
+        <v>3796</v>
       </c>
       <c r="AH117">
-        <v>1396</v>
+        <v>1727</v>
       </c>
       <c r="AI117">
-        <v>21026</v>
+        <v>12893</v>
       </c>
       <c r="AJ117">
-        <v>6863</v>
+        <v>1333</v>
       </c>
       <c r="AK117">
-        <v>19836</v>
+        <v>45318</v>
       </c>
       <c r="AL117">
         <v>6165</v>
@@ -16782,22 +16500,22 @@
         <v>2707</v>
       </c>
       <c r="AF118">
-        <v>3184</v>
+        <v>5497</v>
       </c>
       <c r="AG118">
-        <v>2172</v>
+        <v>3813</v>
       </c>
       <c r="AH118">
-        <v>1484</v>
+        <v>1684</v>
       </c>
       <c r="AI118">
-        <v>19678</v>
+        <v>12751</v>
       </c>
       <c r="AJ118">
-        <v>7003</v>
+        <v>1355</v>
       </c>
       <c r="AK118">
-        <v>16804</v>
+        <v>41950</v>
       </c>
       <c r="AL118">
         <v>5999</v>
@@ -16955,22 +16673,22 @@
         <v>2723</v>
       </c>
       <c r="AF119">
-        <v>2711</v>
+        <v>5913</v>
       </c>
       <c r="AG119">
-        <v>2406</v>
+        <v>4085</v>
       </c>
       <c r="AH119">
-        <v>1663</v>
+        <v>1828</v>
       </c>
       <c r="AI119">
-        <v>21937</v>
+        <v>13825</v>
       </c>
       <c r="AJ119">
-        <v>7054</v>
+        <v>1411</v>
       </c>
       <c r="AK119">
-        <v>17315</v>
+        <v>40419</v>
       </c>
       <c r="AL119">
         <v>5931</v>
@@ -17128,22 +16846,22 @@
         <v>2759</v>
       </c>
       <c r="AF120">
-        <v>3540</v>
+        <v>6533</v>
       </c>
       <c r="AG120">
-        <v>2251</v>
+        <v>4639</v>
       </c>
       <c r="AH120">
-        <v>1617</v>
+        <v>1894</v>
       </c>
       <c r="AI120">
-        <v>22030</v>
+        <v>13711</v>
       </c>
       <c r="AJ120">
-        <v>7084</v>
+        <v>1405</v>
       </c>
       <c r="AK120">
-        <v>17400</v>
+        <v>41555</v>
       </c>
       <c r="AL120">
         <v>5921</v>
@@ -17301,22 +17019,22 @@
         <v>2824</v>
       </c>
       <c r="AF121">
-        <v>3502</v>
+        <v>6904</v>
       </c>
       <c r="AG121">
-        <v>2892</v>
+        <v>4911</v>
       </c>
       <c r="AH121">
-        <v>1663</v>
+        <v>1993</v>
       </c>
       <c r="AI121">
-        <v>21558</v>
+        <v>12894</v>
       </c>
       <c r="AJ121">
-        <v>6988</v>
+        <v>1322</v>
       </c>
       <c r="AK121">
-        <v>17348</v>
+        <v>44333</v>
       </c>
       <c r="AL121">
         <v>6017</v>
@@ -17477,22 +17195,22 @@
         <v>2847</v>
       </c>
       <c r="AF122">
-        <v>3586</v>
+        <v>7382</v>
       </c>
       <c r="AG122">
-        <v>2776</v>
+        <v>5227</v>
       </c>
       <c r="AH122">
-        <v>1887</v>
+        <v>2155</v>
       </c>
       <c r="AI122">
-        <v>21049</v>
+        <v>11983</v>
       </c>
       <c r="AJ122">
-        <v>7029</v>
+        <v>1181</v>
       </c>
       <c r="AK122">
-        <v>19376</v>
+        <v>45687</v>
       </c>
       <c r="AL122">
         <v>6147</v>
@@ -17653,22 +17371,22 @@
         <v>2880</v>
       </c>
       <c r="AF123">
-        <v>4149</v>
+        <v>7652</v>
       </c>
       <c r="AG123">
-        <v>3041</v>
+        <v>5421</v>
       </c>
       <c r="AH123">
-        <v>1507</v>
+        <v>2231</v>
       </c>
       <c r="AI123">
-        <v>22048</v>
+        <v>12134</v>
       </c>
       <c r="AJ123">
-        <v>7000</v>
+        <v>1161</v>
       </c>
       <c r="AK123">
-        <v>21629</v>
+        <v>45619</v>
       </c>
       <c r="AL123">
         <v>6045</v>
@@ -17829,22 +17547,22 @@
         <v>2939</v>
       </c>
       <c r="AF124">
-        <v>4232</v>
+        <v>7890</v>
       </c>
       <c r="AG124">
-        <v>2609</v>
+        <v>5552</v>
       </c>
       <c r="AH124">
-        <v>1720</v>
+        <v>2338</v>
       </c>
       <c r="AI124">
-        <v>21903</v>
+        <v>12907</v>
       </c>
       <c r="AJ124">
-        <v>7158</v>
+        <v>1270</v>
       </c>
       <c r="AK124">
-        <v>21006</v>
+        <v>44252</v>
       </c>
       <c r="AL124">
         <v>5952</v>
@@ -18005,22 +17723,22 @@
         <v>2975</v>
       </c>
       <c r="AF125">
-        <v>3829</v>
+        <v>8181</v>
       </c>
       <c r="AG125">
-        <v>2944</v>
+        <v>5732</v>
       </c>
       <c r="AH125">
-        <v>1841</v>
+        <v>2449</v>
       </c>
       <c r="AI125">
-        <v>21386</v>
+        <v>13307</v>
       </c>
       <c r="AJ125">
-        <v>7402</v>
+        <v>1203</v>
       </c>
       <c r="AK125">
-        <v>19046</v>
+        <v>42564</v>
       </c>
       <c r="AL125">
         <v>5946</v>
@@ -18181,22 +17899,22 @@
         <v>2993</v>
       </c>
       <c r="AF126">
-        <v>4198</v>
+        <v>8698</v>
       </c>
       <c r="AG126">
-        <v>2864</v>
+        <v>6181</v>
       </c>
       <c r="AH126">
-        <v>2030</v>
+        <v>2517</v>
       </c>
       <c r="AI126">
-        <v>20629</v>
+        <v>12852</v>
       </c>
       <c r="AJ126">
-        <v>7219</v>
+        <v>1226</v>
       </c>
       <c r="AK126">
-        <v>17379</v>
+        <v>40828</v>
       </c>
       <c r="AL126">
         <v>5913</v>
@@ -18357,22 +18075,22 @@
         <v>3034</v>
       </c>
       <c r="AF127">
-        <v>4462</v>
+        <v>9286</v>
       </c>
       <c r="AG127">
-        <v>3686</v>
+        <v>6628</v>
       </c>
       <c r="AH127">
-        <v>2045</v>
+        <v>2658</v>
       </c>
       <c r="AI127">
-        <v>22766</v>
+        <v>12925</v>
       </c>
       <c r="AJ127">
-        <v>7474</v>
+        <v>1148</v>
       </c>
       <c r="AK127">
-        <v>19026</v>
+        <v>41819</v>
       </c>
       <c r="AL127">
         <v>6087</v>
@@ -18533,22 +18251,22 @@
         <v>3055</v>
       </c>
       <c r="AF128">
-        <v>4333</v>
+        <v>9610</v>
       </c>
       <c r="AG128">
-        <v>3286</v>
+        <v>6880</v>
       </c>
       <c r="AH128">
-        <v>2232</v>
+        <v>2730</v>
       </c>
       <c r="AI128">
-        <v>22830</v>
+        <v>11575</v>
       </c>
       <c r="AJ128">
-        <v>7490</v>
+        <v>1017</v>
       </c>
       <c r="AK128">
-        <v>16431</v>
+        <v>45016</v>
       </c>
       <c r="AL128">
         <v>6322</v>
@@ -18709,22 +18427,22 @@
         <v>3106</v>
       </c>
       <c r="AF129">
-        <v>4953</v>
+        <v>9689</v>
       </c>
       <c r="AG129">
-        <v>3820</v>
+        <v>6811</v>
       </c>
       <c r="AH129">
-        <v>2260</v>
+        <v>2878</v>
       </c>
       <c r="AI129">
-        <v>21396</v>
+        <v>11296</v>
       </c>
       <c r="AJ129">
-        <v>7694</v>
+        <v>953</v>
       </c>
       <c r="AK129">
-        <v>19688</v>
+        <v>46706</v>
       </c>
       <c r="AL129">
         <v>6478</v>
@@ -18885,22 +18603,22 @@
         <v>3146</v>
       </c>
       <c r="AF130">
-        <v>5308</v>
+        <v>10002</v>
       </c>
       <c r="AG130">
-        <v>3898</v>
+        <v>7079</v>
       </c>
       <c r="AH130">
-        <v>2489</v>
+        <v>2923</v>
       </c>
       <c r="AI130">
-        <v>21676</v>
+        <v>10698</v>
       </c>
       <c r="AJ130">
-        <v>7207</v>
+        <v>940</v>
       </c>
       <c r="AK130">
-        <v>22552</v>
+        <v>46943</v>
       </c>
       <c r="AL130">
         <v>6379</v>
@@ -19061,22 +18779,22 @@
         <v>3190</v>
       </c>
       <c r="AF131">
-        <v>4490</v>
+        <v>10083</v>
       </c>
       <c r="AG131">
-        <v>3972</v>
+        <v>7170</v>
       </c>
       <c r="AH131">
-        <v>2512</v>
+        <v>2913</v>
       </c>
       <c r="AI131">
-        <v>21631</v>
+        <v>11188</v>
       </c>
       <c r="AJ131">
-        <v>7366</v>
+        <v>930</v>
       </c>
       <c r="AK131">
-        <v>19705</v>
+        <v>46338</v>
       </c>
       <c r="AL131">
         <v>6353</v>
@@ -19237,22 +18955,22 @@
         <v>3212</v>
       </c>
       <c r="AF132">
-        <v>5408</v>
+        <v>10410</v>
       </c>
       <c r="AG132">
-        <v>4269</v>
+        <v>7415</v>
       </c>
       <c r="AH132">
-        <v>2507</v>
+        <v>2995</v>
       </c>
       <c r="AI132">
-        <v>23344</v>
+        <v>11726</v>
       </c>
       <c r="AJ132">
-        <v>7422</v>
+        <v>977</v>
       </c>
       <c r="AK132">
-        <v>21533</v>
+        <v>45740</v>
       </c>
       <c r="AL132">
         <v>6405</v>
@@ -19413,22 +19131,22 @@
         <v>3300</v>
       </c>
       <c r="AF133">
-        <v>6211</v>
+        <v>10405</v>
       </c>
       <c r="AG133">
-        <v>3936</v>
+        <v>7352</v>
       </c>
       <c r="AH133">
-        <v>2479</v>
+        <v>3053</v>
       </c>
       <c r="AI133">
-        <v>23245</v>
+        <v>12066</v>
       </c>
       <c r="AJ133">
-        <v>7696</v>
+        <v>984</v>
       </c>
       <c r="AK133">
-        <v>18883</v>
+        <v>43566</v>
       </c>
       <c r="AL133">
         <v>6370</v>
@@ -19589,22 +19307,22 @@
         <v>3371</v>
       </c>
       <c r="AF134">
-        <v>6117</v>
+        <v>10569</v>
       </c>
       <c r="AG134">
-        <v>4205</v>
+        <v>7425</v>
       </c>
       <c r="AH134">
-        <v>2824</v>
+        <v>3144</v>
       </c>
       <c r="AI134">
-        <v>22663</v>
+        <v>11402</v>
       </c>
       <c r="AJ134">
-        <v>7560</v>
+        <v>949</v>
       </c>
       <c r="AK134">
-        <v>21427</v>
+        <v>43615</v>
       </c>
       <c r="AL134">
         <v>6334</v>
@@ -19765,22 +19483,22 @@
         <v>3487</v>
       </c>
       <c r="AF135">
-        <v>4810</v>
+        <v>10471</v>
       </c>
       <c r="AG135">
-        <v>5156</v>
+        <v>7367</v>
       </c>
       <c r="AH135">
-        <v>2822</v>
+        <v>3104</v>
       </c>
       <c r="AI135">
-        <v>23733</v>
+        <v>10586</v>
       </c>
       <c r="AJ135">
-        <v>7700</v>
+        <v>853</v>
       </c>
       <c r="AK135">
-        <v>20688</v>
+        <v>45585</v>
       </c>
       <c r="AL135">
         <v>6583</v>
@@ -19887,22 +19605,22 @@
         <v>3498</v>
       </c>
       <c r="AF136">
-        <v>5520</v>
+        <v>10457</v>
       </c>
       <c r="AG136">
-        <v>4954</v>
+        <v>7288</v>
       </c>
       <c r="AH136">
-        <v>2664</v>
+        <v>3169</v>
       </c>
       <c r="AI136">
-        <v>22798</v>
+        <v>10759</v>
       </c>
       <c r="AJ136">
-        <v>7080</v>
+        <v>865</v>
       </c>
       <c r="AK136">
-        <v>20552</v>
+        <v>46389</v>
       </c>
       <c r="AL136">
         <v>6666</v>
@@ -20009,22 +19727,22 @@
         <v>3535</v>
       </c>
       <c r="AF137">
-        <v>4881</v>
+        <v>10632</v>
       </c>
       <c r="AG137">
-        <v>4869</v>
+        <v>7416</v>
       </c>
       <c r="AH137">
-        <v>2783</v>
+        <v>3216</v>
       </c>
       <c r="AI137">
-        <v>23969</v>
+        <v>10479</v>
       </c>
       <c r="AJ137">
-        <v>7800</v>
+        <v>896</v>
       </c>
       <c r="AK137">
-        <v>19201</v>
+        <v>46216</v>
       </c>
       <c r="AL137">
         <v>6693</v>
@@ -20131,22 +19849,22 @@
         <v>3731</v>
       </c>
       <c r="AF138">
-        <v>5642</v>
+        <v>10658</v>
       </c>
       <c r="AG138">
-        <v>4622</v>
+        <v>7395</v>
       </c>
       <c r="AH138">
-        <v>2402</v>
+        <v>3263</v>
       </c>
       <c r="AI138">
-        <v>22622</v>
+        <v>10831</v>
       </c>
       <c r="AJ138">
-        <v>7198</v>
+        <v>966</v>
       </c>
       <c r="AK138">
-        <v>19134</v>
+        <v>46495</v>
       </c>
       <c r="AL138">
         <v>6658</v>
@@ -20253,22 +19971,22 @@
         <v>3746</v>
       </c>
       <c r="AF139">
-        <v>5776</v>
+        <v>10592</v>
       </c>
       <c r="AG139">
-        <v>4350</v>
+        <v>7180</v>
       </c>
       <c r="AH139">
-        <v>2699</v>
+        <v>3412</v>
       </c>
       <c r="AI139">
-        <v>23411</v>
+        <v>11072</v>
       </c>
       <c r="AJ139">
-        <v>7648</v>
+        <v>943</v>
       </c>
       <c r="AK139">
-        <v>21542</v>
+        <v>44709</v>
       </c>
       <c r="AL139">
         <v>6661</v>
@@ -20375,22 +20093,22 @@
         <v>3781</v>
       </c>
       <c r="AF140">
-        <v>6087</v>
+        <v>10569</v>
       </c>
       <c r="AG140">
-        <v>4991</v>
+        <v>7372</v>
       </c>
       <c r="AH140">
-        <v>2888</v>
+        <v>3197</v>
       </c>
       <c r="AI140">
-        <v>22604</v>
+        <v>11167</v>
       </c>
       <c r="AJ140">
-        <v>7326</v>
+        <v>1004</v>
       </c>
       <c r="AK140">
-        <v>20093</v>
+        <v>43479</v>
       </c>
       <c r="AL140">
         <v>6633</v>
@@ -20473,22 +20191,22 @@
         <v>10848</v>
       </c>
       <c r="AF141">
-        <v>6068</v>
+        <v>10848</v>
       </c>
       <c r="AG141">
-        <v>4701</v>
+        <v>7567</v>
       </c>
       <c r="AH141">
-        <v>2811</v>
+        <v>3281</v>
       </c>
       <c r="AI141">
-        <v>22294</v>
+        <v>11461</v>
       </c>
       <c r="AJ141">
-        <v>7543</v>
+        <v>1088</v>
       </c>
       <c r="AK141">
-        <v>21265</v>
+        <v>43802</v>
       </c>
       <c r="AL141">
         <v>6654</v>
@@ -20595,22 +20313,22 @@
         <v>3987</v>
       </c>
       <c r="AF142">
-        <v>6149</v>
+        <v>10893</v>
       </c>
       <c r="AG142">
-        <v>5074</v>
+        <v>7564</v>
       </c>
       <c r="AH142">
-        <v>2704</v>
+        <v>3329</v>
       </c>
       <c r="AI142">
-        <v>24411</v>
+        <v>10520</v>
       </c>
       <c r="AJ142">
-        <v>7421</v>
+        <v>1031</v>
       </c>
       <c r="AK142">
-        <v>18985</v>
+        <v>45635</v>
       </c>
       <c r="AL142">
         <v>6794</v>
@@ -20726,22 +20444,22 @@
         <v>4440</v>
       </c>
       <c r="AF143">
-        <v>5578</v>
+        <v>8858</v>
       </c>
       <c r="AG143">
-        <v>4389</v>
+        <v>5698</v>
       </c>
       <c r="AH143">
-        <v>2833</v>
+        <v>3160</v>
       </c>
       <c r="AI143">
-        <v>23230</v>
+        <v>13476</v>
       </c>
       <c r="AJ143">
-        <v>8490</v>
+        <v>1267</v>
       </c>
       <c r="AK143">
-        <v>18371</v>
+        <v>36109</v>
       </c>
       <c r="AL143">
         <v>3758</v>
@@ -20848,22 +20566,22 @@
         <v>4677</v>
       </c>
       <c r="AF144">
-        <v>6819</v>
+        <v>10036</v>
       </c>
       <c r="AG144">
-        <v>5005</v>
+        <v>6808</v>
       </c>
       <c r="AH144">
-        <v>3203</v>
+        <v>3228</v>
       </c>
       <c r="AI144">
-        <v>23305</v>
+        <v>14441</v>
       </c>
       <c r="AJ144">
-        <v>8149</v>
+        <v>1396</v>
       </c>
       <c r="AK144">
-        <v>21375</v>
+        <v>44728</v>
       </c>
       <c r="AL144">
         <v>6552</v>
@@ -20970,22 +20688,22 @@
         <v>5011</v>
       </c>
       <c r="AF145">
-        <v>6619</v>
+        <v>9827</v>
       </c>
       <c r="AG145">
-        <v>5275</v>
+        <v>6647</v>
       </c>
       <c r="AH145">
-        <v>3466</v>
+        <v>3180</v>
       </c>
       <c r="AI145">
-        <v>23988</v>
+        <v>13837</v>
       </c>
       <c r="AJ145">
-        <v>8136</v>
+        <v>1261</v>
       </c>
       <c r="AK145">
-        <v>22689</v>
+        <v>47982</v>
       </c>
       <c r="AL145">
         <v>6932</v>
@@ -21089,22 +20807,22 @@
         <v>5201</v>
       </c>
       <c r="AF146">
-        <v>7429</v>
+        <v>10075</v>
       </c>
       <c r="AG146">
-        <v>4976</v>
+        <v>6849</v>
       </c>
       <c r="AH146">
-        <v>3463</v>
+        <v>3209</v>
       </c>
       <c r="AI146">
-        <v>24608</v>
+        <v>11443</v>
       </c>
       <c r="AJ146">
-        <v>7823</v>
+        <v>1243</v>
       </c>
       <c r="AK146">
-        <v>26080</v>
+        <v>23089</v>
       </c>
       <c r="AL146">
         <v>7225</v>
@@ -21211,22 +20929,22 @@
         <v>5257</v>
       </c>
       <c r="AF147">
-        <v>7050</v>
+        <v>9794</v>
       </c>
       <c r="AG147">
-        <v>5578</v>
+        <v>6424</v>
       </c>
       <c r="AH147">
-        <v>3104</v>
+        <v>3352</v>
       </c>
       <c r="AI147">
-        <v>24823</v>
+        <v>12279</v>
       </c>
       <c r="AJ147">
-        <v>7454</v>
+        <v>1353</v>
       </c>
       <c r="AK147">
-        <v>22680</v>
+        <v>41548</v>
       </c>
       <c r="AL147">
         <v>6989</v>
@@ -21324,22 +21042,22 @@
         <v>5544</v>
       </c>
       <c r="AF148">
-        <v>6756</v>
+        <v>9593</v>
       </c>
       <c r="AG148">
-        <v>5549</v>
+        <v>6457</v>
       </c>
       <c r="AH148">
-        <v>3019</v>
+        <v>3136</v>
       </c>
       <c r="AI148">
-        <v>25912</v>
+        <v>13444</v>
       </c>
       <c r="AJ148">
-        <v>7563</v>
+        <v>1348</v>
       </c>
       <c r="AK148">
-        <v>21252</v>
+        <v>45221</v>
       </c>
       <c r="AL148">
         <v>7319</v>
@@ -21413,22 +21131,22 @@
         <v>9595</v>
       </c>
       <c r="AF149">
-        <v>7211</v>
+        <v>9595</v>
       </c>
       <c r="AG149">
-        <v>4496</v>
+        <v>6508</v>
       </c>
       <c r="AH149">
-        <v>3204</v>
+        <v>3087</v>
       </c>
       <c r="AI149">
-        <v>25305</v>
+        <v>12201</v>
       </c>
       <c r="AJ149">
-        <v>7791</v>
+        <v>1362</v>
       </c>
       <c r="AK149">
-        <v>19873</v>
+        <v>42902</v>
       </c>
       <c r="AL149">
         <v>7418</v>
@@ -21493,22 +21211,22 @@
         <v>9296</v>
       </c>
       <c r="AF150">
-        <v>7364</v>
+        <v>9296</v>
       </c>
       <c r="AG150">
-        <v>5503</v>
+        <v>6141</v>
       </c>
       <c r="AH150">
-        <v>3126</v>
+        <v>3036</v>
       </c>
       <c r="AI150">
-        <v>25475</v>
+        <v>10906</v>
       </c>
       <c r="AJ150">
-        <v>7651</v>
+        <v>1080</v>
       </c>
       <c r="AK150">
-        <v>19378</v>
+        <v>43593</v>
       </c>
       <c r="AL150">
         <v>6893</v>
@@ -21517,13 +21235,13 @@
         <v>6195</v>
       </c>
       <c r="BF150">
-        <v>468</v>
+        <v>416</v>
       </c>
       <c r="BG150">
-        <v>505</v>
+        <v>491</v>
       </c>
       <c r="BH150">
-        <v>92.67</v>
+        <v>84.73</v>
       </c>
       <c r="BI150">
         <v>29677668</v>
@@ -21582,22 +21300,22 @@
         <v>9336</v>
       </c>
       <c r="AF151">
-        <v>7554</v>
+        <v>9336</v>
       </c>
       <c r="AG151">
-        <v>4362</v>
+        <v>6165</v>
       </c>
       <c r="AH151">
-        <v>3174</v>
+        <v>3117</v>
       </c>
       <c r="AI151">
-        <v>25143</v>
+        <v>11412</v>
       </c>
       <c r="AJ151">
-        <v>7090</v>
+        <v>1112</v>
       </c>
       <c r="AK151">
-        <v>24760</v>
+        <v>34808</v>
       </c>
       <c r="AL151">
         <v>6898</v>
@@ -21644,22 +21362,22 @@
         <v>8969</v>
       </c>
       <c r="AF152">
-        <v>6163</v>
+        <v>8969</v>
       </c>
       <c r="AG152">
-        <v>5007</v>
+        <v>5794</v>
       </c>
       <c r="AH152">
-        <v>3553</v>
+        <v>3115</v>
       </c>
       <c r="AI152">
-        <v>25310</v>
+        <v>11674</v>
       </c>
       <c r="AJ152">
-        <v>7314</v>
+        <v>1170</v>
       </c>
       <c r="AK152">
-        <v>21894</v>
+        <v>43105</v>
       </c>
       <c r="AL152">
         <v>6169</v>

</xml_diff>

<commit_message>
fix county capitalization & add stats
</commit_message>
<xml_diff>
--- a/combined-datasets/state.xlsx
+++ b/combined-datasets/state.xlsx
@@ -23715,6 +23715,24 @@
       <c r="I173">
         <v>-1062</v>
       </c>
+      <c r="J173">
+        <v>-17.80647436846176</v>
+      </c>
+      <c r="K173">
+        <v>-4.717344758484968</v>
+      </c>
+      <c r="L173">
+        <v>9.059966003533305</v>
+      </c>
+      <c r="M173">
+        <v>-24.56136261893969</v>
+      </c>
+      <c r="N173">
+        <v>-16.08077760167679</v>
+      </c>
+      <c r="O173">
+        <v>5.23813023931898</v>
+      </c>
       <c r="P173">
         <v>4668028</v>
       </c>
@@ -23797,6 +23815,24 @@
       </c>
       <c r="I174">
         <v>-4999</v>
+      </c>
+      <c r="J174">
+        <v>-15.59344646964976</v>
+      </c>
+      <c r="K174">
+        <v>-8.191235382655181</v>
+      </c>
+      <c r="L174">
+        <v>4.111819123521552</v>
+      </c>
+      <c r="M174">
+        <v>-23.87434664806574</v>
+      </c>
+      <c r="N174">
+        <v>-16.53832600696317</v>
+      </c>
+      <c r="O174">
+        <v>4.764358597857199</v>
       </c>
       <c r="P174">
         <v>4696650</v>

</xml_diff>